<commit_message>
Update bookmarklets_v2/WLA Web Page SEO Toolset/WLA Web Page SEO Toolset.js
</commit_message>
<xml_diff>
--- a/family_tree_project/alto_family/excel/Alto Family Tree.xlsx
+++ b/family_tree_project/alto_family/excel/Alto Family Tree.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29721"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -400,7 +400,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mmm\ d\,\ yyyy\ \(ddd\)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -492,6 +492,15 @@
   </cellStyles>
   <dxfs count="21">
     <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
       <border>
         <left style="thin">
           <color auto="1"/>
@@ -508,15 +517,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -589,10 +589,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{10E5E3DB-85CE-4457-908D-EB99FC4303A8}" name="Family" displayName="Family" ref="A5:O84" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="A5:O84" xr:uid="{10E5E3DB-85CE-4457-908D-EB99FC4303A8}"/>
@@ -630,10 +626,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9098B77B-4DD1-4DFD-BE95-AAA1FFD03E58}" name="Lookup_Gender" displayName="Lookup_Gender" ref="A3:A5" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9098B77B-4DD1-4DFD-BE95-AAA1FFD03E58}" name="Lookup_Gender" displayName="Lookup_Gender" ref="A3:A5" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
   <autoFilter ref="A3:A5" xr:uid="{9098B77B-4DD1-4DFD-BE95-AAA1FFD03E58}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{63BAEA8C-3836-42F0-ADBC-BA6F9A119A97}" name="Gender" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{63BAEA8C-3836-42F0-ADBC-BA6F9A119A97}" name="Gender" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -965,22 +961,22 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" customWidth="1"/>
-    <col min="2" max="2" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="20.77734375" style="2" customWidth="1"/>
-    <col min="7" max="9" width="20.77734375" customWidth="1"/>
-    <col min="10" max="10" width="30.6640625" customWidth="1"/>
-    <col min="11" max="11" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="20.7109375" style="2" customWidth="1"/>
+    <col min="7" max="9" width="20.7109375" customWidth="1"/>
+    <col min="10" max="10" width="30.7109375" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -988,7 +984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -998,7 +994,7 @@
       </c>
       <c r="C3" s="3"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -1045,7 +1041,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15">
       <c r="A6">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>1</v>
@@ -1094,7 +1090,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15">
       <c r="A7">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>2</v>
@@ -1143,7 +1139,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15">
       <c r="A8">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>3</v>
@@ -1192,7 +1188,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15">
       <c r="A9">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>4</v>
@@ -1239,7 +1235,7 @@
         <v>92 years, 1 months, 23 days</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15">
       <c r="A10">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>5</v>
@@ -1284,7 +1280,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15">
       <c r="A11">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>6</v>
@@ -1331,7 +1327,7 @@
         <v>90 years, 0 months, 17 days</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15">
       <c r="A12">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>7</v>
@@ -1376,7 +1372,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15">
       <c r="A13">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>8</v>
@@ -1423,7 +1419,7 @@
         <v>85 years, 7 months, 10 days</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15">
       <c r="A14">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>9</v>
@@ -1468,7 +1464,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15">
       <c r="A15">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>10</v>
@@ -1515,7 +1511,7 @@
         <v>83 years, 6 months, 29 days</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15">
       <c r="A16">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>11</v>
@@ -1560,7 +1556,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15">
       <c r="A17">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>12</v>
@@ -1605,7 +1601,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15">
       <c r="A18">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>13</v>
@@ -1652,7 +1648,7 @@
         <v>78 years, 1 months, 24 days</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15">
       <c r="A19">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>14</v>
@@ -1701,7 +1697,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15">
       <c r="A20">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>15</v>
@@ -1746,7 +1742,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15">
       <c r="A21">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>16</v>
@@ -1793,7 +1789,7 @@
         <v>71 years, 10 months, 15 days</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15">
       <c r="A22">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>17</v>
@@ -1838,7 +1834,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15">
       <c r="A23">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>18</v>
@@ -1883,7 +1879,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15">
       <c r="A24">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>19</v>
@@ -1930,7 +1926,7 @@
         <v>69 years, 4 months, 16 days</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15">
       <c r="A25">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>20</v>
@@ -1975,7 +1971,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15">
       <c r="A26">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>21</v>
@@ -2020,7 +2016,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15">
       <c r="A27">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>22</v>
@@ -2065,7 +2061,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15">
       <c r="A28">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>23</v>
@@ -2110,7 +2106,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15">
       <c r="A29">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>24</v>
@@ -2155,7 +2151,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15">
       <c r="A30">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>25</v>
@@ -2200,7 +2196,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15">
       <c r="A31">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>26</v>
@@ -2245,7 +2241,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15">
       <c r="A32">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>27</v>
@@ -2290,7 +2286,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15">
       <c r="A33">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>28</v>
@@ -2335,7 +2331,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15">
       <c r="A34">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>29</v>
@@ -2380,7 +2376,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15">
       <c r="A35">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>30</v>
@@ -2425,7 +2421,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15">
       <c r="A36">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>31</v>
@@ -2470,7 +2466,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15">
       <c r="A37">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>32</v>
@@ -2515,7 +2511,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15">
       <c r="A38">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>33</v>
@@ -2560,7 +2556,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15">
       <c r="A39">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>34</v>
@@ -2605,7 +2601,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15">
       <c r="A40">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>35</v>
@@ -2650,7 +2646,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:15">
       <c r="A41">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>36</v>
@@ -2695,7 +2691,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:15">
       <c r="A42">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>37</v>
@@ -2740,7 +2736,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:15">
       <c r="A43">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>38</v>
@@ -2785,7 +2781,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:15">
       <c r="A44">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>39</v>
@@ -2830,7 +2826,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:15">
       <c r="A45">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>40</v>
@@ -2875,7 +2871,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:15">
       <c r="A46">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>41</v>
@@ -2920,7 +2916,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:15">
       <c r="A47">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>42</v>
@@ -2965,7 +2961,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:15">
       <c r="A48">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>43</v>
@@ -3010,7 +3006,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:15">
       <c r="A49">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>44</v>
@@ -3055,7 +3051,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:15">
       <c r="A50">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>45</v>
@@ -3100,7 +3096,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:15">
       <c r="A51">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>46</v>
@@ -3145,7 +3141,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:15">
       <c r="A52">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>47</v>
@@ -3190,7 +3186,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:15">
       <c r="A53">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>48</v>
@@ -3235,7 +3231,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:15">
       <c r="A54">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>49</v>
@@ -3280,7 +3276,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:15">
       <c r="A55">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>50</v>
@@ -3325,7 +3321,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:15">
       <c r="A56">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>51</v>
@@ -3370,7 +3366,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:15">
       <c r="A57">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>52</v>
@@ -3415,7 +3411,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:15">
       <c r="A58">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>53</v>
@@ -3460,7 +3456,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:15">
       <c r="A59">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>54</v>
@@ -3505,7 +3501,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:15">
       <c r="A60">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>55</v>
@@ -3550,7 +3546,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:15">
       <c r="A61">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>56</v>
@@ -3595,7 +3591,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:15">
       <c r="A62">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>57</v>
@@ -3640,7 +3636,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:15">
       <c r="A63">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>58</v>
@@ -3685,7 +3681,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:15">
       <c r="A64">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>59</v>
@@ -3730,7 +3726,7 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:15">
       <c r="A65">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>60</v>
@@ -3775,7 +3771,7 @@
         <v/>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:15">
       <c r="A66">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>61</v>
@@ -3820,7 +3816,7 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:15">
       <c r="A67">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>62</v>
@@ -3865,7 +3861,7 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:15">
       <c r="A68">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>63</v>
@@ -3910,7 +3906,7 @@
         <v/>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:15">
       <c r="A69">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>64</v>
@@ -3955,7 +3951,7 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:15">
       <c r="A70">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>65</v>
@@ -4000,7 +3996,7 @@
         <v/>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:15">
       <c r="A71">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>66</v>
@@ -4045,7 +4041,7 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:15">
       <c r="A72">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>67</v>
@@ -4090,7 +4086,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:15">
       <c r="A73">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>68</v>
@@ -4135,7 +4131,7 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:15">
       <c r="A74">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>69</v>
@@ -4180,7 +4176,7 @@
         <v/>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:15">
       <c r="A75">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>70</v>
@@ -4225,7 +4221,7 @@
         <v/>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:15">
       <c r="A76">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>71</v>
@@ -4270,7 +4266,7 @@
         <v/>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:15">
       <c r="A77">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>72</v>
@@ -4315,7 +4311,7 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:15">
       <c r="A78">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>73</v>
@@ -4360,7 +4356,7 @@
         <v/>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:15">
       <c r="A79">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>74</v>
@@ -4405,7 +4401,7 @@
         <v/>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:15">
       <c r="A80">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>75</v>
@@ -4450,7 +4446,7 @@
         <v/>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:15">
       <c r="A81">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>76</v>
@@ -4495,7 +4491,7 @@
         <v/>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:15">
       <c r="A82">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>77</v>
@@ -4540,7 +4536,7 @@
         <v/>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:15">
       <c r="A83">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>78</v>
@@ -4585,7 +4581,7 @@
         <v/>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:15">
       <c r="A84">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>79</v>
@@ -4630,7 +4626,7 @@
         <v/>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:15">
       <c r="B85" s="5"/>
       <c r="C85" s="5"/>
       <c r="D85" s="5"/>
@@ -4641,7 +4637,7 @@
       <c r="I85" s="5"/>
       <c r="J85" s="5"/>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:15">
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
       <c r="D86" s="5"/>
@@ -4652,7 +4648,7 @@
       <c r="I86" s="5"/>
       <c r="J86" s="5"/>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:15">
       <c r="B87" s="5"/>
       <c r="C87" s="5"/>
       <c r="D87" s="5"/>
@@ -4663,7 +4659,7 @@
       <c r="I87" s="5"/>
       <c r="J87" s="5"/>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:15">
       <c r="B88" s="5"/>
       <c r="C88" s="5"/>
       <c r="D88" s="5"/>
@@ -4674,7 +4670,7 @@
       <c r="I88" s="5"/>
       <c r="J88" s="5"/>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:15">
       <c r="B89" s="5"/>
       <c r="C89" s="5"/>
       <c r="D89" s="5"/>
@@ -4685,7 +4681,7 @@
       <c r="I89" s="5"/>
       <c r="J89" s="5"/>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:15">
       <c r="B90" s="5"/>
       <c r="C90" s="5"/>
       <c r="D90" s="5"/>
@@ -4696,7 +4692,7 @@
       <c r="I90" s="5"/>
       <c r="J90" s="5"/>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:15">
       <c r="B91" s="5"/>
       <c r="C91" s="5"/>
       <c r="D91" s="5"/>
@@ -4707,7 +4703,7 @@
       <c r="I91" s="5"/>
       <c r="J91" s="5"/>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:15">
       <c r="B92" s="5"/>
       <c r="C92" s="5"/>
       <c r="D92" s="5"/>
@@ -4718,7 +4714,7 @@
       <c r="I92" s="5"/>
       <c r="J92" s="5"/>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:15">
       <c r="B93" s="5"/>
       <c r="C93" s="5"/>
       <c r="D93" s="5"/>
@@ -4729,7 +4725,7 @@
       <c r="I93" s="5"/>
       <c r="J93" s="5"/>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:15">
       <c r="B94" s="5"/>
       <c r="C94" s="5"/>
       <c r="D94" s="5"/>
@@ -4740,7 +4736,7 @@
       <c r="I94" s="5"/>
       <c r="J94" s="5"/>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:15">
       <c r="B95" s="5"/>
       <c r="C95" s="5"/>
       <c r="D95" s="5"/>
@@ -4751,7 +4747,7 @@
       <c r="I95" s="5"/>
       <c r="J95" s="5"/>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:15">
       <c r="B96" s="5"/>
       <c r="C96" s="5"/>
       <c r="D96" s="5"/>
@@ -4762,7 +4758,7 @@
       <c r="I96" s="5"/>
       <c r="J96" s="5"/>
     </row>
-    <row r="97" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:10">
       <c r="B97" s="5"/>
       <c r="C97" s="5"/>
       <c r="D97" s="5"/>
@@ -4773,7 +4769,7 @@
       <c r="I97" s="5"/>
       <c r="J97" s="5"/>
     </row>
-    <row r="98" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:10">
       <c r="B98" s="5"/>
       <c r="C98" s="5"/>
       <c r="D98" s="5"/>
@@ -4784,7 +4780,7 @@
       <c r="I98" s="5"/>
       <c r="J98" s="5"/>
     </row>
-    <row r="99" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:10">
       <c r="B99" s="5"/>
       <c r="C99" s="5"/>
       <c r="D99" s="5"/>
@@ -4795,7 +4791,7 @@
       <c r="I99" s="5"/>
       <c r="J99" s="5"/>
     </row>
-    <row r="100" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:10">
       <c r="B100" s="5"/>
       <c r="C100" s="5"/>
       <c r="D100" s="5"/>
@@ -4806,7 +4802,7 @@
       <c r="I100" s="5"/>
       <c r="J100" s="5"/>
     </row>
-    <row r="101" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:10">
       <c r="B101" s="5"/>
       <c r="C101" s="5"/>
       <c r="D101" s="5"/>
@@ -4817,7 +4813,7 @@
       <c r="I101" s="5"/>
       <c r="J101" s="5"/>
     </row>
-    <row r="102" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:10">
       <c r="B102" s="5"/>
       <c r="C102" s="5"/>
       <c r="D102" s="5"/>
@@ -4828,7 +4824,7 @@
       <c r="I102" s="5"/>
       <c r="J102" s="5"/>
     </row>
-    <row r="103" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:10">
       <c r="B103" s="5"/>
       <c r="C103" s="5"/>
       <c r="D103" s="5"/>
@@ -4839,7 +4835,7 @@
       <c r="I103" s="5"/>
       <c r="J103" s="5"/>
     </row>
-    <row r="104" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:10">
       <c r="B104" s="5"/>
       <c r="C104" s="5"/>
       <c r="D104" s="5"/>
@@ -4850,7 +4846,7 @@
       <c r="I104" s="5"/>
       <c r="J104" s="5"/>
     </row>
-    <row r="105" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:10">
       <c r="B105" s="5"/>
       <c r="C105" s="5"/>
       <c r="D105" s="5"/>
@@ -4861,7 +4857,7 @@
       <c r="I105" s="5"/>
       <c r="J105" s="5"/>
     </row>
-    <row r="106" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:10">
       <c r="B106" s="5"/>
       <c r="C106" s="5"/>
       <c r="D106" s="5"/>
@@ -4872,7 +4868,7 @@
       <c r="I106" s="5"/>
       <c r="J106" s="5"/>
     </row>
-    <row r="107" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:10">
       <c r="B107" s="5"/>
       <c r="C107" s="5"/>
       <c r="D107" s="5"/>
@@ -4883,7 +4879,7 @@
       <c r="I107" s="5"/>
       <c r="J107" s="5"/>
     </row>
-    <row r="108" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:10">
       <c r="B108" s="5"/>
       <c r="C108" s="5"/>
       <c r="D108" s="5"/>
@@ -4894,7 +4890,7 @@
       <c r="I108" s="5"/>
       <c r="J108" s="5"/>
     </row>
-    <row r="109" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:10">
       <c r="B109" s="5"/>
       <c r="C109" s="5"/>
       <c r="D109" s="5"/>
@@ -4905,7 +4901,7 @@
       <c r="I109" s="5"/>
       <c r="J109" s="5"/>
     </row>
-    <row r="110" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:10">
       <c r="B110" s="5"/>
       <c r="C110" s="5"/>
       <c r="D110" s="5"/>
@@ -4916,7 +4912,7 @@
       <c r="I110" s="5"/>
       <c r="J110" s="5"/>
     </row>
-    <row r="111" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:10">
       <c r="B111" s="5"/>
       <c r="C111" s="5"/>
       <c r="D111" s="5"/>
@@ -4927,7 +4923,7 @@
       <c r="I111" s="5"/>
       <c r="J111" s="5"/>
     </row>
-    <row r="112" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:10">
       <c r="B112" s="5"/>
       <c r="C112" s="5"/>
       <c r="D112" s="5"/>
@@ -4938,7 +4934,7 @@
       <c r="I112" s="5"/>
       <c r="J112" s="5"/>
     </row>
-    <row r="113" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:10">
       <c r="B113" s="5"/>
       <c r="C113" s="5"/>
       <c r="D113" s="5"/>
@@ -4949,7 +4945,7 @@
       <c r="I113" s="5"/>
       <c r="J113" s="5"/>
     </row>
-    <row r="114" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:10">
       <c r="B114" s="5"/>
       <c r="C114" s="5"/>
       <c r="D114" s="5"/>
@@ -4960,7 +4956,7 @@
       <c r="I114" s="5"/>
       <c r="J114" s="5"/>
     </row>
-    <row r="115" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:10">
       <c r="B115" s="5"/>
       <c r="C115" s="5"/>
       <c r="D115" s="5"/>
@@ -4971,7 +4967,7 @@
       <c r="I115" s="5"/>
       <c r="J115" s="5"/>
     </row>
-    <row r="116" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:10">
       <c r="B116" s="5"/>
       <c r="C116" s="5"/>
       <c r="D116" s="5"/>
@@ -4982,7 +4978,7 @@
       <c r="I116" s="5"/>
       <c r="J116" s="5"/>
     </row>
-    <row r="117" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:10">
       <c r="B117" s="5"/>
       <c r="C117" s="5"/>
       <c r="D117" s="5"/>
@@ -4993,7 +4989,7 @@
       <c r="I117" s="5"/>
       <c r="J117" s="5"/>
     </row>
-    <row r="118" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:10">
       <c r="B118" s="5"/>
       <c r="C118" s="5"/>
       <c r="D118" s="5"/>
@@ -5004,7 +5000,7 @@
       <c r="I118" s="5"/>
       <c r="J118" s="5"/>
     </row>
-    <row r="119" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:10">
       <c r="B119" s="5"/>
       <c r="C119" s="5"/>
       <c r="D119" s="5"/>
@@ -5015,7 +5011,7 @@
       <c r="I119" s="5"/>
       <c r="J119" s="5"/>
     </row>
-    <row r="120" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:10">
       <c r="B120" s="5"/>
       <c r="C120" s="5"/>
       <c r="D120" s="5"/>
@@ -5026,7 +5022,7 @@
       <c r="I120" s="5"/>
       <c r="J120" s="5"/>
     </row>
-    <row r="121" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:10">
       <c r="B121" s="5"/>
       <c r="C121" s="5"/>
       <c r="D121" s="5"/>
@@ -5037,7 +5033,7 @@
       <c r="I121" s="5"/>
       <c r="J121" s="5"/>
     </row>
-    <row r="122" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:10">
       <c r="B122" s="5"/>
       <c r="C122" s="5"/>
       <c r="D122" s="5"/>
@@ -5048,7 +5044,7 @@
       <c r="I122" s="5"/>
       <c r="J122" s="5"/>
     </row>
-    <row r="123" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:10">
       <c r="B123" s="5"/>
       <c r="C123" s="5"/>
       <c r="D123" s="5"/>
@@ -5059,7 +5055,7 @@
       <c r="I123" s="5"/>
       <c r="J123" s="5"/>
     </row>
-    <row r="124" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:10">
       <c r="B124" s="5"/>
       <c r="C124" s="5"/>
       <c r="D124" s="5"/>
@@ -5070,7 +5066,7 @@
       <c r="I124" s="5"/>
       <c r="J124" s="5"/>
     </row>
-    <row r="125" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:10">
       <c r="B125" s="5"/>
       <c r="C125" s="5"/>
       <c r="D125" s="5"/>
@@ -5081,7 +5077,7 @@
       <c r="I125" s="5"/>
       <c r="J125" s="5"/>
     </row>
-    <row r="126" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:10">
       <c r="B126" s="5"/>
       <c r="C126" s="5"/>
       <c r="D126" s="5"/>
@@ -5092,7 +5088,7 @@
       <c r="I126" s="5"/>
       <c r="J126" s="5"/>
     </row>
-    <row r="127" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:10">
       <c r="B127" s="5"/>
       <c r="C127" s="5"/>
       <c r="D127" s="5"/>
@@ -5103,7 +5099,7 @@
       <c r="I127" s="5"/>
       <c r="J127" s="5"/>
     </row>
-    <row r="128" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:10">
       <c r="B128" s="5"/>
       <c r="C128" s="5"/>
       <c r="D128" s="5"/>
@@ -5114,7 +5110,7 @@
       <c r="I128" s="5"/>
       <c r="J128" s="5"/>
     </row>
-    <row r="129" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:10">
       <c r="B129" s="5"/>
       <c r="C129" s="5"/>
       <c r="D129" s="5"/>
@@ -5125,7 +5121,7 @@
       <c r="I129" s="5"/>
       <c r="J129" s="5"/>
     </row>
-    <row r="130" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:10">
       <c r="B130" s="5"/>
       <c r="C130" s="5"/>
       <c r="D130" s="5"/>
@@ -5136,7 +5132,7 @@
       <c r="I130" s="5"/>
       <c r="J130" s="5"/>
     </row>
-    <row r="131" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:10">
       <c r="B131" s="5"/>
       <c r="C131" s="5"/>
       <c r="D131" s="5"/>
@@ -5147,7 +5143,7 @@
       <c r="I131" s="5"/>
       <c r="J131" s="5"/>
     </row>
-    <row r="132" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:10">
       <c r="B132" s="5"/>
       <c r="C132" s="5"/>
       <c r="D132" s="5"/>
@@ -5158,7 +5154,7 @@
       <c r="I132" s="5"/>
       <c r="J132" s="5"/>
     </row>
-    <row r="133" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:10">
       <c r="B133" s="5"/>
       <c r="C133" s="5"/>
       <c r="D133" s="5"/>
@@ -5169,7 +5165,7 @@
       <c r="I133" s="5"/>
       <c r="J133" s="5"/>
     </row>
-    <row r="134" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:10">
       <c r="B134" s="5"/>
       <c r="C134" s="5"/>
       <c r="D134" s="5"/>
@@ -5180,7 +5176,7 @@
       <c r="I134" s="5"/>
       <c r="J134" s="5"/>
     </row>
-    <row r="135" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:10">
       <c r="B135" s="5"/>
       <c r="C135" s="5"/>
       <c r="D135" s="5"/>
@@ -5191,7 +5187,7 @@
       <c r="I135" s="5"/>
       <c r="J135" s="5"/>
     </row>
-    <row r="136" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:10">
       <c r="B136" s="5"/>
       <c r="C136" s="5"/>
       <c r="D136" s="5"/>
@@ -5202,7 +5198,7 @@
       <c r="I136" s="5"/>
       <c r="J136" s="5"/>
     </row>
-    <row r="137" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:10">
       <c r="B137" s="5"/>
       <c r="C137" s="5"/>
       <c r="D137" s="5"/>
@@ -5213,7 +5209,7 @@
       <c r="I137" s="5"/>
       <c r="J137" s="5"/>
     </row>
-    <row r="138" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:10">
       <c r="B138" s="5"/>
       <c r="C138" s="5"/>
       <c r="D138" s="5"/>
@@ -5224,7 +5220,7 @@
       <c r="I138" s="5"/>
       <c r="J138" s="5"/>
     </row>
-    <row r="139" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:10">
       <c r="B139" s="5"/>
       <c r="C139" s="5"/>
       <c r="D139" s="5"/>
@@ -5235,7 +5231,7 @@
       <c r="I139" s="5"/>
       <c r="J139" s="5"/>
     </row>
-    <row r="140" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:10">
       <c r="B140" s="5"/>
       <c r="C140" s="5"/>
       <c r="D140" s="5"/>
@@ -5246,7 +5242,7 @@
       <c r="I140" s="5"/>
       <c r="J140" s="5"/>
     </row>
-    <row r="141" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:10">
       <c r="B141" s="5"/>
       <c r="C141" s="5"/>
       <c r="D141" s="5"/>
@@ -5257,7 +5253,7 @@
       <c r="I141" s="5"/>
       <c r="J141" s="5"/>
     </row>
-    <row r="142" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:10">
       <c r="B142" s="5"/>
       <c r="C142" s="5"/>
       <c r="D142" s="5"/>
@@ -5268,7 +5264,7 @@
       <c r="I142" s="5"/>
       <c r="J142" s="5"/>
     </row>
-    <row r="143" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:10">
       <c r="B143" s="5"/>
       <c r="C143" s="5"/>
       <c r="D143" s="5"/>
@@ -5279,7 +5275,7 @@
       <c r="I143" s="5"/>
       <c r="J143" s="5"/>
     </row>
-    <row r="144" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:10">
       <c r="B144" s="5"/>
       <c r="C144" s="5"/>
       <c r="D144" s="5"/>
@@ -5290,7 +5286,7 @@
       <c r="I144" s="5"/>
       <c r="J144" s="5"/>
     </row>
-    <row r="145" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:10">
       <c r="B145" s="5"/>
       <c r="C145" s="5"/>
       <c r="D145" s="5"/>
@@ -5301,7 +5297,7 @@
       <c r="I145" s="5"/>
       <c r="J145" s="5"/>
     </row>
-    <row r="146" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:10">
       <c r="B146" s="5"/>
       <c r="C146" s="5"/>
       <c r="D146" s="5"/>
@@ -5312,7 +5308,7 @@
       <c r="I146" s="5"/>
       <c r="J146" s="5"/>
     </row>
-    <row r="147" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:10">
       <c r="B147" s="5"/>
       <c r="C147" s="5"/>
       <c r="D147" s="5"/>
@@ -5323,7 +5319,7 @@
       <c r="I147" s="5"/>
       <c r="J147" s="5"/>
     </row>
-    <row r="148" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:10">
       <c r="B148" s="5"/>
       <c r="C148" s="5"/>
       <c r="D148" s="5"/>
@@ -5334,7 +5330,7 @@
       <c r="I148" s="5"/>
       <c r="J148" s="5"/>
     </row>
-    <row r="149" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:10">
       <c r="B149" s="5"/>
       <c r="C149" s="5"/>
       <c r="D149" s="5"/>
@@ -5345,7 +5341,7 @@
       <c r="I149" s="5"/>
       <c r="J149" s="5"/>
     </row>
-    <row r="150" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:10">
       <c r="B150" s="5"/>
       <c r="C150" s="5"/>
       <c r="D150" s="5"/>
@@ -5356,7 +5352,7 @@
       <c r="I150" s="5"/>
       <c r="J150" s="5"/>
     </row>
-    <row r="151" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:10">
       <c r="B151" s="5"/>
       <c r="C151" s="5"/>
       <c r="D151" s="5"/>
@@ -5367,7 +5363,7 @@
       <c r="I151" s="5"/>
       <c r="J151" s="5"/>
     </row>
-    <row r="152" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:10">
       <c r="B152" s="5"/>
       <c r="C152" s="5"/>
       <c r="D152" s="5"/>
@@ -5378,7 +5374,7 @@
       <c r="I152" s="5"/>
       <c r="J152" s="5"/>
     </row>
-    <row r="153" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:10">
       <c r="B153" s="5"/>
       <c r="C153" s="5"/>
       <c r="D153" s="5"/>
@@ -5389,7 +5385,7 @@
       <c r="I153" s="5"/>
       <c r="J153" s="5"/>
     </row>
-    <row r="154" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="154" spans="2:10">
       <c r="B154" s="5"/>
       <c r="C154" s="5"/>
       <c r="D154" s="5"/>
@@ -5400,7 +5396,7 @@
       <c r="I154" s="5"/>
       <c r="J154" s="5"/>
     </row>
-    <row r="155" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="155" spans="2:10">
       <c r="B155" s="5"/>
       <c r="C155" s="5"/>
       <c r="D155" s="5"/>
@@ -5411,7 +5407,7 @@
       <c r="I155" s="5"/>
       <c r="J155" s="5"/>
     </row>
-    <row r="156" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="156" spans="2:10">
       <c r="B156" s="5"/>
       <c r="C156" s="5"/>
       <c r="D156" s="5"/>
@@ -5422,7 +5418,7 @@
       <c r="I156" s="5"/>
       <c r="J156" s="5"/>
     </row>
-    <row r="157" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="157" spans="2:10">
       <c r="B157" s="5"/>
       <c r="C157" s="5"/>
       <c r="D157" s="5"/>
@@ -5433,7 +5429,7 @@
       <c r="I157" s="5"/>
       <c r="J157" s="5"/>
     </row>
-    <row r="158" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="158" spans="2:10">
       <c r="B158" s="5"/>
       <c r="C158" s="5"/>
       <c r="D158" s="5"/>
@@ -5444,7 +5440,7 @@
       <c r="I158" s="5"/>
       <c r="J158" s="5"/>
     </row>
-    <row r="159" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="159" spans="2:10">
       <c r="B159" s="5"/>
       <c r="C159" s="5"/>
       <c r="D159" s="5"/>
@@ -5455,7 +5451,7 @@
       <c r="I159" s="5"/>
       <c r="J159" s="5"/>
     </row>
-    <row r="160" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="160" spans="2:10">
       <c r="B160" s="5"/>
       <c r="C160" s="5"/>
       <c r="D160" s="5"/>
@@ -5466,7 +5462,7 @@
       <c r="I160" s="5"/>
       <c r="J160" s="5"/>
     </row>
-    <row r="161" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="161" spans="2:10">
       <c r="B161" s="5"/>
       <c r="C161" s="5"/>
       <c r="D161" s="5"/>
@@ -5477,7 +5473,7 @@
       <c r="I161" s="5"/>
       <c r="J161" s="5"/>
     </row>
-    <row r="162" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="162" spans="2:10">
       <c r="B162" s="5"/>
       <c r="C162" s="5"/>
       <c r="D162" s="5"/>
@@ -5488,7 +5484,7 @@
       <c r="I162" s="5"/>
       <c r="J162" s="5"/>
     </row>
-    <row r="163" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="163" spans="2:10">
       <c r="B163" s="5"/>
       <c r="C163" s="5"/>
       <c r="D163" s="5"/>
@@ -5499,7 +5495,7 @@
       <c r="I163" s="5"/>
       <c r="J163" s="5"/>
     </row>
-    <row r="164" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="164" spans="2:10">
       <c r="B164" s="5"/>
       <c r="C164" s="5"/>
       <c r="D164" s="5"/>
@@ -5510,7 +5506,7 @@
       <c r="I164" s="5"/>
       <c r="J164" s="5"/>
     </row>
-    <row r="165" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="165" spans="2:10">
       <c r="B165" s="5"/>
       <c r="C165" s="5"/>
       <c r="D165" s="5"/>
@@ -5521,7 +5517,7 @@
       <c r="I165" s="5"/>
       <c r="J165" s="5"/>
     </row>
-    <row r="166" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="166" spans="2:10">
       <c r="B166" s="5"/>
       <c r="C166" s="5"/>
       <c r="D166" s="5"/>
@@ -5532,7 +5528,7 @@
       <c r="I166" s="5"/>
       <c r="J166" s="5"/>
     </row>
-    <row r="167" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="167" spans="2:10">
       <c r="B167" s="5"/>
       <c r="C167" s="5"/>
       <c r="D167" s="5"/>
@@ -5543,7 +5539,7 @@
       <c r="I167" s="5"/>
       <c r="J167" s="5"/>
     </row>
-    <row r="168" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="168" spans="2:10">
       <c r="B168" s="5"/>
       <c r="C168" s="5"/>
       <c r="D168" s="5"/>
@@ -5554,7 +5550,7 @@
       <c r="I168" s="5"/>
       <c r="J168" s="5"/>
     </row>
-    <row r="169" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="169" spans="2:10">
       <c r="B169" s="5"/>
       <c r="C169" s="5"/>
       <c r="D169" s="5"/>
@@ -5565,7 +5561,7 @@
       <c r="I169" s="5"/>
       <c r="J169" s="5"/>
     </row>
-    <row r="170" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="170" spans="2:10">
       <c r="B170" s="5"/>
       <c r="C170" s="5"/>
       <c r="D170" s="5"/>
@@ -5576,7 +5572,7 @@
       <c r="I170" s="5"/>
       <c r="J170" s="5"/>
     </row>
-    <row r="171" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="171" spans="2:10">
       <c r="B171" s="5"/>
       <c r="C171" s="5"/>
       <c r="D171" s="5"/>
@@ -5587,7 +5583,7 @@
       <c r="I171" s="5"/>
       <c r="J171" s="5"/>
     </row>
-    <row r="172" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="172" spans="2:10">
       <c r="B172" s="5"/>
       <c r="C172" s="5"/>
       <c r="D172" s="5"/>
@@ -5598,7 +5594,7 @@
       <c r="I172" s="5"/>
       <c r="J172" s="5"/>
     </row>
-    <row r="173" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="173" spans="2:10">
       <c r="B173" s="5"/>
       <c r="C173" s="5"/>
       <c r="D173" s="5"/>
@@ -5609,7 +5605,7 @@
       <c r="I173" s="5"/>
       <c r="J173" s="5"/>
     </row>
-    <row r="174" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="174" spans="2:10">
       <c r="B174" s="5"/>
       <c r="C174" s="5"/>
       <c r="D174" s="5"/>
@@ -5620,7 +5616,7 @@
       <c r="I174" s="5"/>
       <c r="J174" s="5"/>
     </row>
-    <row r="175" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="175" spans="2:10">
       <c r="B175" s="5"/>
       <c r="C175" s="5"/>
       <c r="D175" s="5"/>
@@ -5631,7 +5627,7 @@
       <c r="I175" s="5"/>
       <c r="J175" s="5"/>
     </row>
-    <row r="176" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="176" spans="2:10">
       <c r="B176" s="5"/>
       <c r="C176" s="5"/>
       <c r="D176" s="5"/>
@@ -5642,7 +5638,7 @@
       <c r="I176" s="5"/>
       <c r="J176" s="5"/>
     </row>
-    <row r="177" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="177" spans="2:10">
       <c r="B177" s="5"/>
       <c r="C177" s="5"/>
       <c r="D177" s="5"/>
@@ -5653,7 +5649,7 @@
       <c r="I177" s="5"/>
       <c r="J177" s="5"/>
     </row>
-    <row r="178" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="178" spans="2:10">
       <c r="B178" s="5"/>
       <c r="C178" s="5"/>
       <c r="D178" s="5"/>
@@ -5664,7 +5660,7 @@
       <c r="I178" s="5"/>
       <c r="J178" s="5"/>
     </row>
-    <row r="179" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="179" spans="2:10">
       <c r="B179" s="5"/>
       <c r="C179" s="5"/>
       <c r="D179" s="5"/>
@@ -5675,7 +5671,7 @@
       <c r="I179" s="5"/>
       <c r="J179" s="5"/>
     </row>
-    <row r="180" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="180" spans="2:10">
       <c r="B180" s="5"/>
       <c r="C180" s="5"/>
       <c r="D180" s="5"/>
@@ -5686,7 +5682,7 @@
       <c r="I180" s="5"/>
       <c r="J180" s="5"/>
     </row>
-    <row r="181" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="181" spans="2:10">
       <c r="B181" s="5"/>
       <c r="C181" s="5"/>
       <c r="D181" s="5"/>
@@ -5697,7 +5693,7 @@
       <c r="I181" s="5"/>
       <c r="J181" s="5"/>
     </row>
-    <row r="182" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="182" spans="2:10">
       <c r="B182" s="5"/>
       <c r="C182" s="5"/>
       <c r="D182" s="5"/>
@@ -5708,7 +5704,7 @@
       <c r="I182" s="5"/>
       <c r="J182" s="5"/>
     </row>
-    <row r="183" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="183" spans="2:10">
       <c r="B183" s="5"/>
       <c r="C183" s="5"/>
       <c r="D183" s="5"/>
@@ -5719,7 +5715,7 @@
       <c r="I183" s="5"/>
       <c r="J183" s="5"/>
     </row>
-    <row r="184" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="184" spans="2:10">
       <c r="B184" s="5"/>
       <c r="C184" s="5"/>
       <c r="D184" s="5"/>
@@ -5730,7 +5726,7 @@
       <c r="I184" s="5"/>
       <c r="J184" s="5"/>
     </row>
-    <row r="185" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="185" spans="2:10">
       <c r="B185" s="5"/>
       <c r="C185" s="5"/>
       <c r="D185" s="5"/>
@@ -5741,7 +5737,7 @@
       <c r="I185" s="5"/>
       <c r="J185" s="5"/>
     </row>
-    <row r="186" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="186" spans="2:10">
       <c r="B186" s="5"/>
       <c r="C186" s="5"/>
       <c r="D186" s="5"/>
@@ -5752,7 +5748,7 @@
       <c r="I186" s="5"/>
       <c r="J186" s="5"/>
     </row>
-    <row r="187" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="187" spans="2:10">
       <c r="B187" s="5"/>
       <c r="C187" s="5"/>
       <c r="D187" s="5"/>
@@ -5763,7 +5759,7 @@
       <c r="I187" s="5"/>
       <c r="J187" s="5"/>
     </row>
-    <row r="188" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="188" spans="2:10">
       <c r="B188" s="5"/>
       <c r="C188" s="5"/>
       <c r="D188" s="5"/>
@@ -5774,7 +5770,7 @@
       <c r="I188" s="5"/>
       <c r="J188" s="5"/>
     </row>
-    <row r="189" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="189" spans="2:10">
       <c r="B189" s="5"/>
       <c r="C189" s="5"/>
       <c r="D189" s="5"/>
@@ -5785,7 +5781,7 @@
       <c r="I189" s="5"/>
       <c r="J189" s="5"/>
     </row>
-    <row r="190" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="190" spans="2:10">
       <c r="B190" s="5"/>
       <c r="C190" s="5"/>
       <c r="D190" s="5"/>
@@ -5796,7 +5792,7 @@
       <c r="I190" s="5"/>
       <c r="J190" s="5"/>
     </row>
-    <row r="191" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="191" spans="2:10">
       <c r="B191" s="5"/>
       <c r="C191" s="5"/>
       <c r="D191" s="5"/>
@@ -5807,7 +5803,7 @@
       <c r="I191" s="5"/>
       <c r="J191" s="5"/>
     </row>
-    <row r="192" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="192" spans="2:10">
       <c r="B192" s="5"/>
       <c r="C192" s="5"/>
       <c r="D192" s="5"/>
@@ -5818,7 +5814,7 @@
       <c r="I192" s="5"/>
       <c r="J192" s="5"/>
     </row>
-    <row r="193" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="193" spans="2:10">
       <c r="B193" s="5"/>
       <c r="C193" s="5"/>
       <c r="D193" s="5"/>
@@ -5829,7 +5825,7 @@
       <c r="I193" s="5"/>
       <c r="J193" s="5"/>
     </row>
-    <row r="194" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="194" spans="2:10">
       <c r="B194" s="5"/>
       <c r="C194" s="5"/>
       <c r="D194" s="5"/>
@@ -5840,7 +5836,7 @@
       <c r="I194" s="5"/>
       <c r="J194" s="5"/>
     </row>
-    <row r="195" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="195" spans="2:10">
       <c r="B195" s="5"/>
       <c r="C195" s="5"/>
       <c r="D195" s="5"/>
@@ -5851,7 +5847,7 @@
       <c r="I195" s="5"/>
       <c r="J195" s="5"/>
     </row>
-    <row r="196" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="196" spans="2:10">
       <c r="B196" s="5"/>
       <c r="C196" s="5"/>
       <c r="D196" s="5"/>
@@ -5862,7 +5858,7 @@
       <c r="I196" s="5"/>
       <c r="J196" s="5"/>
     </row>
-    <row r="197" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="197" spans="2:10">
       <c r="B197" s="5"/>
       <c r="C197" s="5"/>
       <c r="D197" s="5"/>
@@ -5873,7 +5869,7 @@
       <c r="I197" s="5"/>
       <c r="J197" s="5"/>
     </row>
-    <row r="198" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="198" spans="2:10">
       <c r="B198" s="5"/>
       <c r="C198" s="5"/>
       <c r="D198" s="5"/>
@@ -5884,7 +5880,7 @@
       <c r="I198" s="5"/>
       <c r="J198" s="5"/>
     </row>
-    <row r="199" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="199" spans="2:10">
       <c r="B199" s="5"/>
       <c r="C199" s="5"/>
       <c r="D199" s="5"/>
@@ -5895,7 +5891,7 @@
       <c r="I199" s="5"/>
       <c r="J199" s="5"/>
     </row>
-    <row r="200" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="200" spans="2:10">
       <c r="B200" s="5"/>
       <c r="C200" s="5"/>
       <c r="D200" s="5"/>
@@ -5906,7 +5902,7 @@
       <c r="I200" s="5"/>
       <c r="J200" s="5"/>
     </row>
-    <row r="201" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="201" spans="2:10">
       <c r="B201" s="5"/>
       <c r="C201" s="5"/>
       <c r="D201" s="5"/>
@@ -5917,7 +5913,7 @@
       <c r="I201" s="5"/>
       <c r="J201" s="5"/>
     </row>
-    <row r="202" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="202" spans="2:10">
       <c r="B202" s="5"/>
       <c r="C202" s="5"/>
       <c r="D202" s="5"/>
@@ -5928,7 +5924,7 @@
       <c r="I202" s="5"/>
       <c r="J202" s="5"/>
     </row>
-    <row r="203" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="203" spans="2:10">
       <c r="B203" s="5"/>
       <c r="C203" s="5"/>
       <c r="D203" s="5"/>
@@ -5939,7 +5935,7 @@
       <c r="I203" s="5"/>
       <c r="J203" s="5"/>
     </row>
-    <row r="204" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="204" spans="2:10">
       <c r="B204" s="5"/>
       <c r="C204" s="5"/>
       <c r="D204" s="5"/>
@@ -5950,7 +5946,7 @@
       <c r="I204" s="5"/>
       <c r="J204" s="5"/>
     </row>
-    <row r="205" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="205" spans="2:10">
       <c r="B205" s="5"/>
       <c r="C205" s="5"/>
       <c r="D205" s="5"/>
@@ -5993,22 +5989,22 @@
       <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12">
       <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
@@ -6046,7 +6042,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12">
       <c r="A6" cm="1">
         <f t="array" ref="A6:A84">Family[PersonID]</f>
         <v>1</v>
@@ -6096,7 +6092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12">
       <c r="A7">
         <v>2</v>
       </c>
@@ -6135,7 +6131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12">
       <c r="A8">
         <v>3</v>
       </c>
@@ -6174,7 +6170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12">
       <c r="A9">
         <v>4</v>
       </c>
@@ -6213,7 +6209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12">
       <c r="A10">
         <v>5</v>
       </c>
@@ -6252,7 +6248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12">
       <c r="A11">
         <v>6</v>
       </c>
@@ -6291,7 +6287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12">
       <c r="A12">
         <v>7</v>
       </c>
@@ -6330,7 +6326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12">
       <c r="A13">
         <v>8</v>
       </c>
@@ -6369,7 +6365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12">
       <c r="A14">
         <v>9</v>
       </c>
@@ -6408,7 +6404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12">
       <c r="A15">
         <v>10</v>
       </c>
@@ -6447,7 +6443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12">
       <c r="A16">
         <v>11</v>
       </c>
@@ -6486,7 +6482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12">
       <c r="A17">
         <v>12</v>
       </c>
@@ -6525,7 +6521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12">
       <c r="A18">
         <v>13</v>
       </c>
@@ -6564,7 +6560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12">
       <c r="A19">
         <v>14</v>
       </c>
@@ -6603,7 +6599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12">
       <c r="A20">
         <v>15</v>
       </c>
@@ -6642,7 +6638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12">
       <c r="A21">
         <v>16</v>
       </c>
@@ -6681,7 +6677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12">
       <c r="A22">
         <v>17</v>
       </c>
@@ -6720,7 +6716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12">
       <c r="A23">
         <v>18</v>
       </c>
@@ -6759,7 +6755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12">
       <c r="A24">
         <v>19</v>
       </c>
@@ -6798,7 +6794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12">
       <c r="A25">
         <v>20</v>
       </c>
@@ -6837,7 +6833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12">
       <c r="A26">
         <v>21</v>
       </c>
@@ -6876,7 +6872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12">
       <c r="A27">
         <v>22</v>
       </c>
@@ -6915,7 +6911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12">
       <c r="A28">
         <v>23</v>
       </c>
@@ -6954,7 +6950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12">
       <c r="A29">
         <v>24</v>
       </c>
@@ -6993,7 +6989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12">
       <c r="A30">
         <v>25</v>
       </c>
@@ -7032,7 +7028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12">
       <c r="A31">
         <v>26</v>
       </c>
@@ -7071,7 +7067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12">
       <c r="A32">
         <v>27</v>
       </c>
@@ -7110,7 +7106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12">
       <c r="A33">
         <v>28</v>
       </c>
@@ -7149,7 +7145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12">
       <c r="A34">
         <v>29</v>
       </c>
@@ -7188,7 +7184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12">
       <c r="A35">
         <v>30</v>
       </c>
@@ -7227,7 +7223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12">
       <c r="A36">
         <v>31</v>
       </c>
@@ -7266,7 +7262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12">
       <c r="A37">
         <v>32</v>
       </c>
@@ -7305,7 +7301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12">
       <c r="A38">
         <v>33</v>
       </c>
@@ -7344,7 +7340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12">
       <c r="A39">
         <v>34</v>
       </c>
@@ -7383,7 +7379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12">
       <c r="A40">
         <v>35</v>
       </c>
@@ -7422,7 +7418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12">
       <c r="A41">
         <v>36</v>
       </c>
@@ -7461,7 +7457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12">
       <c r="A42">
         <v>37</v>
       </c>
@@ -7500,7 +7496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12">
       <c r="A43">
         <v>38</v>
       </c>
@@ -7539,7 +7535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12">
       <c r="A44">
         <v>39</v>
       </c>
@@ -7578,7 +7574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12">
       <c r="A45">
         <v>40</v>
       </c>
@@ -7617,7 +7613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12">
       <c r="A46">
         <v>41</v>
       </c>
@@ -7656,7 +7652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12">
       <c r="A47">
         <v>42</v>
       </c>
@@ -7695,7 +7691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12">
       <c r="A48">
         <v>43</v>
       </c>
@@ -7734,7 +7730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12">
       <c r="A49">
         <v>44</v>
       </c>
@@ -7773,7 +7769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12">
       <c r="A50">
         <v>45</v>
       </c>
@@ -7812,7 +7808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12">
       <c r="A51">
         <v>46</v>
       </c>
@@ -7851,7 +7847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12">
       <c r="A52">
         <v>47</v>
       </c>
@@ -7890,7 +7886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12">
       <c r="A53">
         <v>48</v>
       </c>
@@ -7929,7 +7925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12">
       <c r="A54">
         <v>49</v>
       </c>
@@ -7968,7 +7964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12">
       <c r="A55">
         <v>50</v>
       </c>
@@ -8007,7 +8003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12">
       <c r="A56">
         <v>51</v>
       </c>
@@ -8046,7 +8042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12">
       <c r="A57">
         <v>52</v>
       </c>
@@ -8085,7 +8081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12">
       <c r="A58">
         <v>53</v>
       </c>
@@ -8124,7 +8120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12">
       <c r="A59">
         <v>54</v>
       </c>
@@ -8163,7 +8159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12">
       <c r="A60">
         <v>55</v>
       </c>
@@ -8202,7 +8198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12">
       <c r="A61">
         <v>56</v>
       </c>
@@ -8241,7 +8237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12">
       <c r="A62">
         <v>57</v>
       </c>
@@ -8280,7 +8276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12">
       <c r="A63">
         <v>58</v>
       </c>
@@ -8319,7 +8315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12">
       <c r="A64">
         <v>59</v>
       </c>
@@ -8358,7 +8354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12">
       <c r="A65">
         <v>60</v>
       </c>
@@ -8397,7 +8393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12">
       <c r="A66">
         <v>61</v>
       </c>
@@ -8436,7 +8432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12">
       <c r="A67">
         <v>62</v>
       </c>
@@ -8475,7 +8471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12">
       <c r="A68">
         <v>63</v>
       </c>
@@ -8514,7 +8510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12">
       <c r="A69">
         <v>64</v>
       </c>
@@ -8553,7 +8549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12">
       <c r="A70">
         <v>65</v>
       </c>
@@ -8592,7 +8588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12">
       <c r="A71">
         <v>66</v>
       </c>
@@ -8631,7 +8627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:12">
       <c r="A72">
         <v>67</v>
       </c>
@@ -8670,7 +8666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:12">
       <c r="A73">
         <v>68</v>
       </c>
@@ -8709,7 +8705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:12">
       <c r="A74">
         <v>69</v>
       </c>
@@ -8748,7 +8744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12">
       <c r="A75">
         <v>70</v>
       </c>
@@ -8787,7 +8783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12">
       <c r="A76">
         <v>71</v>
       </c>
@@ -8826,7 +8822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:12">
       <c r="A77">
         <v>72</v>
       </c>
@@ -8865,7 +8861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:12">
       <c r="A78">
         <v>73</v>
       </c>
@@ -8904,7 +8900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:12">
       <c r="A79">
         <v>74</v>
       </c>
@@ -8943,7 +8939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:12">
       <c r="A80">
         <v>75</v>
       </c>
@@ -8982,7 +8978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:12">
       <c r="A81">
         <v>76</v>
       </c>
@@ -9021,7 +9017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:12">
       <c r="A82">
         <v>77</v>
       </c>
@@ -9060,7 +9056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:12">
       <c r="A83">
         <v>78</v>
       </c>
@@ -9099,7 +9095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:12">
       <c r="A84">
         <v>79</v>
       </c>
@@ -9141,7 +9137,7 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="z2qPucUrqzpAbNrSN+cTXqXL9VmvHlBebf7zJLZukSo935FG2MWtQHQaAHBYBjvhorIZyzPuXgxNE9xi36mPtA==" saltValue="RQEcPLaOesrjkBOnJxq8Pw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="A6:L10000">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>NOT(ISBLANK(A6))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9160,17 +9156,17 @@
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -9178,12 +9174,12 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Update Alto Family Tree
</commit_message>
<xml_diff>
--- a/family_tree_project/alto_family/excel/Alto Family Tree.xlsx
+++ b/family_tree_project/alto_family/excel/Alto Family Tree.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29721"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/48fcbf0fe29d15ca/Documents/Personal/My Personal Projects/GitHub/washingtonalto.github.io/family_tree_project/alto_family/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{28C1A374-CA4E-49F8-9C0F-2E90EAC04F0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{343435BD-2150-4E02-8912-3CCD08FAD1F3}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="13_ncr:1_{28C1A374-CA4E-49F8-9C0F-2E90EAC04F0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E5002D9-9AAE-44EC-9857-5062D0DD5FC6}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9A1E33E0-BCBF-411C-B6A4-073C88D53E64}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="105">
   <si>
     <t>ALTO FAMILY DATA ENTRY</t>
   </si>
@@ -384,13 +384,22 @@
     <t>Ryder Garland</t>
   </si>
   <si>
-    <t>Alexis Mai Lim</t>
-  </si>
-  <si>
     <t>Lookup_Gender</t>
   </si>
   <si>
     <t>pwd: alto</t>
+  </si>
+  <si>
+    <t>Alexis Mei Lim</t>
+  </si>
+  <si>
+    <t>Samara Jia Lim</t>
+  </si>
+  <si>
+    <t>Tamsyn Jie Lim</t>
+  </si>
+  <si>
+    <t>Nita Nash Wongbandue</t>
   </si>
 </sst>
 </file>
@@ -400,7 +409,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mmm\ d\,\ yyyy\ \(ddd\)"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -472,7 +481,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -486,20 +495,13 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="21">
-    <dxf>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="1" hidden="0"/>
-    </dxf>
     <dxf>
       <border>
         <left style="thin">
@@ -517,6 +519,15 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -590,8 +601,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{10E5E3DB-85CE-4457-908D-EB99FC4303A8}" name="Family" displayName="Family" ref="A5:O84" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
-  <autoFilter ref="A5:O84" xr:uid="{10E5E3DB-85CE-4457-908D-EB99FC4303A8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{10E5E3DB-85CE-4457-908D-EB99FC4303A8}" name="Family" displayName="Family" ref="A5:O87" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+  <autoFilter ref="A5:O87" xr:uid="{10E5E3DB-85CE-4457-908D-EB99FC4303A8}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{9209114C-0460-4570-9D94-C60095FA5745}" name="PersonID" dataDxfId="18">
       <calculatedColumnFormula>ROW()-ROW(Family[[#Headers],[PersonID]])</calculatedColumnFormula>
@@ -626,10 +637,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9098B77B-4DD1-4DFD-BE95-AAA1FFD03E58}" name="Lookup_Gender" displayName="Lookup_Gender" ref="A3:A5" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9098B77B-4DD1-4DFD-BE95-AAA1FFD03E58}" name="Lookup_Gender" displayName="Lookup_Gender" ref="A3:A5" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <autoFilter ref="A3:A5" xr:uid="{9098B77B-4DD1-4DFD-BE95-AAA1FFD03E58}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{63BAEA8C-3836-42F0-ADBC-BA6F9A119A97}" name="Gender" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{63BAEA8C-3836-42F0-ADBC-BA6F9A119A97}" name="Gender" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -955,28 +966,31 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A2:O205"/>
+  <dimension ref="A2:O206"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C36" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="F90" sqref="F90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="20.7109375" style="2" customWidth="1"/>
-    <col min="7" max="9" width="20.7109375" customWidth="1"/>
-    <col min="10" max="10" width="30.7109375" customWidth="1"/>
-    <col min="11" max="11" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="20.6640625" style="2" customWidth="1"/>
+    <col min="7" max="9" width="20.6640625" customWidth="1"/>
+    <col min="10" max="10" width="30.6640625" customWidth="1"/>
+    <col min="11" max="11" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="23.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -984,17 +998,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="3">
         <f ca="1">TODAY()</f>
-        <v>46052</v>
+        <v>46054</v>
       </c>
       <c r="C3" s="3"/>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -1041,7 +1055,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>1</v>
@@ -1090,7 +1104,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>2</v>
@@ -1139,7 +1153,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>3</v>
@@ -1188,7 +1202,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>4</v>
@@ -1232,10 +1246,10 @@
       </c>
       <c r="O9" t="str" cm="1">
         <f t="array" aca="1" ref="O9" ca="1">lambda_currentage(Family[[#This Row],[BirthDate]],Family[[#This Row],[DeathDate]],$B$3)</f>
-        <v>92 years, 1 months, 23 days</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
+        <v>92 years, 1 months, 25 days</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>5</v>
@@ -1280,7 +1294,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>6</v>
@@ -1324,10 +1338,10 @@
       </c>
       <c r="O11" t="str" cm="1">
         <f t="array" aca="1" ref="O11" ca="1">lambda_currentage(Family[[#This Row],[BirthDate]],Family[[#This Row],[DeathDate]],$B$3)</f>
-        <v>90 years, 0 months, 17 days</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15">
+        <v>90 years, 0 months, 19 days</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>7</v>
@@ -1372,7 +1386,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>8</v>
@@ -1416,10 +1430,10 @@
       </c>
       <c r="O13" t="str" cm="1">
         <f t="array" aca="1" ref="O13" ca="1">lambda_currentage(Family[[#This Row],[BirthDate]],Family[[#This Row],[DeathDate]],$B$3)</f>
-        <v>85 years, 7 months, 10 days</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15">
+        <v>85 years, 7 months, 12 days</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>9</v>
@@ -1464,7 +1478,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>10</v>
@@ -1508,10 +1522,10 @@
       </c>
       <c r="O15" t="str" cm="1">
         <f t="array" aca="1" ref="O15" ca="1">lambda_currentage(Family[[#This Row],[BirthDate]],Family[[#This Row],[DeathDate]],$B$3)</f>
-        <v>83 years, 6 months, 29 days</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15">
+        <v>83 years, 7 months, 0 days</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>11</v>
@@ -1556,7 +1570,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>12</v>
@@ -1601,7 +1615,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>13</v>
@@ -1645,10 +1659,10 @@
       </c>
       <c r="O18" t="str" cm="1">
         <f t="array" aca="1" ref="O18" ca="1">lambda_currentage(Family[[#This Row],[BirthDate]],Family[[#This Row],[DeathDate]],$B$3)</f>
-        <v>78 years, 1 months, 24 days</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15">
+        <v>78 years, 1 months, 26 days</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>14</v>
@@ -1697,7 +1711,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>15</v>
@@ -1742,7 +1756,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>16</v>
@@ -1786,10 +1800,10 @@
       </c>
       <c r="O21" t="str" cm="1">
         <f t="array" aca="1" ref="O21" ca="1">lambda_currentage(Family[[#This Row],[BirthDate]],Family[[#This Row],[DeathDate]],$B$3)</f>
-        <v>71 years, 10 months, 15 days</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15">
+        <v>71 years, 10 months, 17 days</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>17</v>
@@ -1834,7 +1848,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>18</v>
@@ -1879,7 +1893,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>19</v>
@@ -1923,10 +1937,10 @@
       </c>
       <c r="O24" t="str" cm="1">
         <f t="array" aca="1" ref="O24" ca="1">lambda_currentage(Family[[#This Row],[BirthDate]],Family[[#This Row],[DeathDate]],$B$3)</f>
-        <v>69 years, 4 months, 16 days</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15">
+        <v>69 years, 4 months, 18 days</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>20</v>
@@ -1971,7 +1985,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>21</v>
@@ -2016,7 +2030,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>22</v>
@@ -2061,7 +2075,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>23</v>
@@ -2106,7 +2120,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>24</v>
@@ -2151,7 +2165,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>25</v>
@@ -2196,7 +2210,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>26</v>
@@ -2241,7 +2255,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>27</v>
@@ -2286,7 +2300,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>28</v>
@@ -2331,7 +2345,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>29</v>
@@ -2376,7 +2390,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>30</v>
@@ -2421,7 +2435,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>31</v>
@@ -2466,7 +2480,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>32</v>
@@ -2511,7 +2525,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>33</v>
@@ -2556,7 +2570,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>34</v>
@@ -2601,7 +2615,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>35</v>
@@ -2646,7 +2660,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>36</v>
@@ -2691,7 +2705,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>37</v>
@@ -2736,7 +2750,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:15">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>38</v>
@@ -2781,7 +2795,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:15">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>39</v>
@@ -2826,7 +2840,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:15">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>40</v>
@@ -2871,7 +2885,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:15">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>41</v>
@@ -2916,7 +2930,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:15">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>42</v>
@@ -2961,7 +2975,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:15">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>43</v>
@@ -3006,7 +3020,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:15">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>44</v>
@@ -3051,7 +3065,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:15">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>45</v>
@@ -3096,7 +3110,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:15">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>46</v>
@@ -3141,7 +3155,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:15">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>47</v>
@@ -3186,7 +3200,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:15">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>48</v>
@@ -3231,7 +3245,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:15">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>49</v>
@@ -3276,7 +3290,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:15">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>50</v>
@@ -3321,7 +3335,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:15">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>51</v>
@@ -3366,7 +3380,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:15">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>52</v>
@@ -3411,7 +3425,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:15">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>53</v>
@@ -3456,7 +3470,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:15">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>54</v>
@@ -3501,7 +3515,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:15">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>55</v>
@@ -3546,7 +3560,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:15">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>56</v>
@@ -3567,7 +3581,7 @@
         <v>39</v>
       </c>
       <c r="I61" s="5" t="s">
-        <v>20</v>
+        <v>104</v>
       </c>
       <c r="J61" s="5"/>
       <c r="K61" cm="1">
@@ -3578,9 +3592,9 @@
         <f t="array" ref="L61">_xlfn.XLOOKUP(Family[[#This Row],[Mother]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
         <v>19</v>
       </c>
-      <c r="M61" t="str" cm="1">
+      <c r="M61" cm="1">
         <f t="array" ref="M61">_xlfn.XLOOKUP(Family[[#This Row],[Spouse]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
-        <v/>
+        <v>57</v>
       </c>
       <c r="N61" t="str" cm="1">
         <f t="array" ref="N61">lambda_lifetimeage(Family[[#This Row],[BirthDate]],Family[[#This Row],[DeathDate]])</f>
@@ -3591,13 +3605,13 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:15">
-      <c r="A62">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A62" s="9">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>57</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>77</v>
+        <v>104</v>
       </c>
       <c r="C62" s="5"/>
       <c r="D62" s="5" t="s">
@@ -3605,44 +3619,40 @@
       </c>
       <c r="E62" s="6"/>
       <c r="F62" s="6"/>
-      <c r="G62" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H62" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="I62" s="5" t="s">
-        <v>20</v>
+      <c r="G62" s="6"/>
+      <c r="H62" s="6"/>
+      <c r="I62" s="6" t="s">
+        <v>76</v>
       </c>
       <c r="J62" s="5"/>
-      <c r="K62" cm="1">
+      <c r="K62" s="9" t="str" cm="1">
         <f t="array" ref="K62">_xlfn.XLOOKUP(Family[[#This Row],[Father]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
-        <v>18</v>
-      </c>
-      <c r="L62" cm="1">
+        <v/>
+      </c>
+      <c r="L62" s="9" t="str" cm="1">
         <f t="array" ref="L62">_xlfn.XLOOKUP(Family[[#This Row],[Mother]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
-        <v>19</v>
-      </c>
-      <c r="M62" t="str" cm="1">
+        <v/>
+      </c>
+      <c r="M62" s="9" cm="1">
         <f t="array" ref="M62">_xlfn.XLOOKUP(Family[[#This Row],[Spouse]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
-        <v/>
-      </c>
-      <c r="N62" t="str" cm="1">
+        <v>56</v>
+      </c>
+      <c r="N62" s="10" t="str" cm="1">
         <f t="array" ref="N62">lambda_lifetimeage(Family[[#This Row],[BirthDate]],Family[[#This Row],[DeathDate]])</f>
         <v/>
       </c>
-      <c r="O62" t="str" cm="1">
+      <c r="O62" s="10" t="str" cm="1">
         <f t="array" ref="O62">lambda_currentage(Family[[#This Row],[BirthDate]],Family[[#This Row],[DeathDate]],$B$3)</f>
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:15">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>58</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C63" s="5"/>
       <c r="D63" s="5" t="s">
@@ -3651,10 +3661,10 @@
       <c r="E63" s="6"/>
       <c r="F63" s="6"/>
       <c r="G63" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="I63" s="5" t="s">
         <v>20</v>
@@ -3662,11 +3672,11 @@
       <c r="J63" s="5"/>
       <c r="K63" cm="1">
         <f t="array" ref="K63">_xlfn.XLOOKUP(Family[[#This Row],[Father]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="L63" cm="1">
         <f t="array" ref="L63">_xlfn.XLOOKUP(Family[[#This Row],[Mother]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="M63" t="str" cm="1">
         <f t="array" ref="M63">_xlfn.XLOOKUP(Family[[#This Row],[Spouse]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
@@ -3681,17 +3691,17 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:15">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A64">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>59</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C64" s="5"/>
       <c r="D64" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E64" s="6"/>
       <c r="F64" s="6"/>
@@ -3726,25 +3736,25 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="1:15">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A65">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>60</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C65" s="5"/>
       <c r="D65" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E65" s="6"/>
       <c r="F65" s="6"/>
       <c r="G65" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I65" s="5" t="s">
         <v>20</v>
@@ -3752,11 +3762,11 @@
       <c r="J65" s="5"/>
       <c r="K65" cm="1">
         <f t="array" ref="K65">_xlfn.XLOOKUP(Family[[#This Row],[Father]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="L65" cm="1">
         <f t="array" ref="L65">_xlfn.XLOOKUP(Family[[#This Row],[Mother]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="M65" t="str" cm="1">
         <f t="array" ref="M65">_xlfn.XLOOKUP(Family[[#This Row],[Spouse]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
@@ -3771,13 +3781,13 @@
         <v/>
       </c>
     </row>
-    <row r="66" spans="1:15">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A66">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>61</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C66" s="5"/>
       <c r="D66" s="5" t="s">
@@ -3786,10 +3796,10 @@
       <c r="E66" s="6"/>
       <c r="F66" s="6"/>
       <c r="G66" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I66" s="5" t="s">
         <v>20</v>
@@ -3797,11 +3807,11 @@
       <c r="J66" s="5"/>
       <c r="K66" cm="1">
         <f t="array" ref="K66">_xlfn.XLOOKUP(Family[[#This Row],[Father]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="L66" cm="1">
         <f t="array" ref="L66">_xlfn.XLOOKUP(Family[[#This Row],[Mother]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="M66" t="str" cm="1">
         <f t="array" ref="M66">_xlfn.XLOOKUP(Family[[#This Row],[Spouse]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
@@ -3816,17 +3826,17 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="1:15">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A67">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>62</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C67" s="5"/>
       <c r="D67" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E67" s="6"/>
       <c r="F67" s="6"/>
@@ -3861,13 +3871,13 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="1:15">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A68">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>63</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C68" s="5"/>
       <c r="D68" s="5" t="s">
@@ -3876,10 +3886,10 @@
       <c r="E68" s="6"/>
       <c r="F68" s="6"/>
       <c r="G68" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H68" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I68" s="5" t="s">
         <v>20</v>
@@ -3887,11 +3897,11 @@
       <c r="J68" s="5"/>
       <c r="K68" cm="1">
         <f t="array" ref="K68">_xlfn.XLOOKUP(Family[[#This Row],[Father]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="L68" cm="1">
         <f t="array" ref="L68">_xlfn.XLOOKUP(Family[[#This Row],[Mother]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="M68" t="str" cm="1">
         <f t="array" ref="M68">_xlfn.XLOOKUP(Family[[#This Row],[Spouse]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
@@ -3906,13 +3916,13 @@
         <v/>
       </c>
     </row>
-    <row r="69" spans="1:15">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A69">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>64</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C69" s="5"/>
       <c r="D69" s="5" t="s">
@@ -3921,10 +3931,10 @@
       <c r="E69" s="6"/>
       <c r="F69" s="6"/>
       <c r="G69" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H69" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I69" s="5" t="s">
         <v>20</v>
@@ -3932,11 +3942,11 @@
       <c r="J69" s="5"/>
       <c r="K69" cm="1">
         <f t="array" ref="K69">_xlfn.XLOOKUP(Family[[#This Row],[Father]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L69" cm="1">
         <f t="array" ref="L69">_xlfn.XLOOKUP(Family[[#This Row],[Mother]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="M69" t="str" cm="1">
         <f t="array" ref="M69">_xlfn.XLOOKUP(Family[[#This Row],[Spouse]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
@@ -3951,17 +3961,17 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="1:15">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A70">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>65</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C70" s="5"/>
       <c r="D70" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E70" s="6"/>
       <c r="F70" s="6"/>
@@ -3996,25 +4006,25 @@
         <v/>
       </c>
     </row>
-    <row r="71" spans="1:15">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A71">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>66</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C71" s="5"/>
       <c r="D71" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E71" s="6"/>
       <c r="F71" s="6"/>
       <c r="G71" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H71" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I71" s="5" t="s">
         <v>20</v>
@@ -4022,11 +4032,11 @@
       <c r="J71" s="5"/>
       <c r="K71" cm="1">
         <f t="array" ref="K71">_xlfn.XLOOKUP(Family[[#This Row],[Father]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L71" cm="1">
         <f t="array" ref="L71">_xlfn.XLOOKUP(Family[[#This Row],[Mother]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="M71" t="str" cm="1">
         <f t="array" ref="M71">_xlfn.XLOOKUP(Family[[#This Row],[Spouse]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
@@ -4041,25 +4051,25 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="1:15">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A72">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>67</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C72" s="5"/>
       <c r="D72" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E72" s="6"/>
       <c r="F72" s="6"/>
       <c r="G72" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="H72" s="5" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="I72" s="5" t="s">
         <v>20</v>
@@ -4067,11 +4077,11 @@
       <c r="J72" s="5"/>
       <c r="K72" cm="1">
         <f t="array" ref="K72">_xlfn.XLOOKUP(Family[[#This Row],[Father]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
-        <v>35</v>
-      </c>
-      <c r="L72" t="str" cm="1">
+        <v>32</v>
+      </c>
+      <c r="L72" cm="1">
         <f t="array" ref="L72">_xlfn.XLOOKUP(Family[[#This Row],[Mother]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
-        <v/>
+        <v>33</v>
       </c>
       <c r="M72" t="str" cm="1">
         <f t="array" ref="M72">_xlfn.XLOOKUP(Family[[#This Row],[Spouse]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
@@ -4086,17 +4096,17 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:15">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A73">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>68</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C73" s="5"/>
       <c r="D73" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E73" s="6"/>
       <c r="F73" s="6"/>
@@ -4131,13 +4141,13 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:15">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A74">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>69</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C74" s="5"/>
       <c r="D74" s="5" t="s">
@@ -4176,25 +4186,25 @@
         <v/>
       </c>
     </row>
-    <row r="75" spans="1:15">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A75">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>70</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C75" s="5"/>
       <c r="D75" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E75" s="6"/>
       <c r="F75" s="6"/>
       <c r="G75" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="H75" s="5" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="I75" s="5" t="s">
         <v>20</v>
@@ -4202,11 +4212,11 @@
       <c r="J75" s="5"/>
       <c r="K75" cm="1">
         <f t="array" ref="K75">_xlfn.XLOOKUP(Family[[#This Row],[Father]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
-        <v>39</v>
-      </c>
-      <c r="L75" cm="1">
+        <v>35</v>
+      </c>
+      <c r="L75" t="str" cm="1">
         <f t="array" ref="L75">_xlfn.XLOOKUP(Family[[#This Row],[Mother]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
-        <v>40</v>
+        <v/>
       </c>
       <c r="M75" t="str" cm="1">
         <f t="array" ref="M75">_xlfn.XLOOKUP(Family[[#This Row],[Spouse]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
@@ -4221,13 +4231,13 @@
         <v/>
       </c>
     </row>
-    <row r="76" spans="1:15">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A76">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>71</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C76" s="5"/>
       <c r="D76" s="5" t="s">
@@ -4236,10 +4246,10 @@
       <c r="E76" s="6"/>
       <c r="F76" s="6"/>
       <c r="G76" s="5" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="H76" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="I76" s="5" t="s">
         <v>20</v>
@@ -4247,11 +4257,11 @@
       <c r="J76" s="5"/>
       <c r="K76" cm="1">
         <f t="array" ref="K76">_xlfn.XLOOKUP(Family[[#This Row],[Father]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="L76" cm="1">
         <f t="array" ref="L76">_xlfn.XLOOKUP(Family[[#This Row],[Mother]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="M76" t="str" cm="1">
         <f t="array" ref="M76">_xlfn.XLOOKUP(Family[[#This Row],[Spouse]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
@@ -4266,17 +4276,17 @@
         <v/>
       </c>
     </row>
-    <row r="77" spans="1:15">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A77">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>72</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C77" s="5"/>
       <c r="D77" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E77" s="6"/>
       <c r="F77" s="6"/>
@@ -4311,25 +4321,25 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="1:15">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A78">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>73</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C78" s="5"/>
       <c r="D78" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E78" s="6"/>
       <c r="F78" s="6"/>
       <c r="G78" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H78" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I78" s="5" t="s">
         <v>20</v>
@@ -4337,11 +4347,11 @@
       <c r="J78" s="5"/>
       <c r="K78" cm="1">
         <f t="array" ref="K78">_xlfn.XLOOKUP(Family[[#This Row],[Father]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L78" cm="1">
         <f t="array" ref="L78">_xlfn.XLOOKUP(Family[[#This Row],[Mother]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M78" t="str" cm="1">
         <f t="array" ref="M78">_xlfn.XLOOKUP(Family[[#This Row],[Spouse]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
@@ -4356,25 +4366,25 @@
         <v/>
       </c>
     </row>
-    <row r="79" spans="1:15">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A79">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>74</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C79" s="5"/>
       <c r="D79" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E79" s="6"/>
       <c r="F79" s="6"/>
       <c r="G79" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H79" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I79" s="5" t="s">
         <v>20</v>
@@ -4382,11 +4392,11 @@
       <c r="J79" s="5"/>
       <c r="K79" cm="1">
         <f t="array" ref="K79">_xlfn.XLOOKUP(Family[[#This Row],[Father]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L79" cm="1">
         <f t="array" ref="L79">_xlfn.XLOOKUP(Family[[#This Row],[Mother]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M79" t="str" cm="1">
         <f t="array" ref="M79">_xlfn.XLOOKUP(Family[[#This Row],[Spouse]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
@@ -4401,13 +4411,13 @@
         <v/>
       </c>
     </row>
-    <row r="80" spans="1:15">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A80">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>75</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C80" s="5"/>
       <c r="D80" s="5" t="s">
@@ -4446,13 +4456,13 @@
         <v/>
       </c>
     </row>
-    <row r="81" spans="1:15">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A81">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>76</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C81" s="5"/>
       <c r="D81" s="5" t="s">
@@ -4491,17 +4501,17 @@
         <v/>
       </c>
     </row>
-    <row r="82" spans="1:15">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A82">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>77</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C82" s="5"/>
       <c r="D82" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E82" s="6"/>
       <c r="F82" s="6"/>
@@ -4536,13 +4546,13 @@
         <v/>
       </c>
     </row>
-    <row r="83" spans="1:15">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A83">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>78</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C83" s="5"/>
       <c r="D83" s="5" t="s">
@@ -4551,22 +4561,22 @@
       <c r="E83" s="6"/>
       <c r="F83" s="6"/>
       <c r="G83" s="5" t="s">
-        <v>20</v>
+        <v>69</v>
       </c>
       <c r="H83" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I83" s="5" t="s">
         <v>20</v>
       </c>
       <c r="J83" s="5"/>
-      <c r="K83" t="str" cm="1">
+      <c r="K83" cm="1">
         <f t="array" ref="K83">_xlfn.XLOOKUP(Family[[#This Row],[Father]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
-        <v/>
+        <v>49</v>
       </c>
       <c r="L83" cm="1">
         <f t="array" ref="L83">_xlfn.XLOOKUP(Family[[#This Row],[Mother]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M83" t="str" cm="1">
         <f t="array" ref="M83">_xlfn.XLOOKUP(Family[[#This Row],[Spouse]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
@@ -4581,13 +4591,13 @@
         <v/>
       </c>
     </row>
-    <row r="84" spans="1:15">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A84">
         <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
         <v>79</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C84" s="5"/>
       <c r="D84" s="5" t="s">
@@ -4596,22 +4606,22 @@
       <c r="E84" s="6"/>
       <c r="F84" s="6"/>
       <c r="G84" s="5" t="s">
-        <v>72</v>
+        <v>20</v>
       </c>
       <c r="H84" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I84" s="5" t="s">
         <v>20</v>
       </c>
       <c r="J84" s="5"/>
-      <c r="K84" cm="1">
+      <c r="K84" t="str" cm="1">
         <f t="array" ref="K84">_xlfn.XLOOKUP(Family[[#This Row],[Father]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
-        <v>52</v>
+        <v/>
       </c>
       <c r="L84" cm="1">
         <f t="array" ref="L84">_xlfn.XLOOKUP(Family[[#This Row],[Mother]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="M84" t="str" cm="1">
         <f t="array" ref="M84">_xlfn.XLOOKUP(Family[[#This Row],[Spouse]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
@@ -4626,40 +4636,146 @@
         <v/>
       </c>
     </row>
-    <row r="85" spans="1:15">
-      <c r="B85" s="5"/>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
+        <v>80</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>101</v>
+      </c>
       <c r="C85" s="5"/>
-      <c r="D85" s="5"/>
-      <c r="E85" s="6"/>
+      <c r="D85" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E85" s="6">
+        <v>41817</v>
+      </c>
       <c r="F85" s="6"/>
-      <c r="G85" s="5"/>
-      <c r="H85" s="5"/>
-      <c r="I85" s="5"/>
+      <c r="G85" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="H85" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="I85" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="J85" s="5"/>
-    </row>
-    <row r="86" spans="1:15">
-      <c r="B86" s="5"/>
+      <c r="K85" cm="1">
+        <f t="array" ref="K85">_xlfn.XLOOKUP(Family[[#This Row],[Father]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
+        <v>52</v>
+      </c>
+      <c r="L85" cm="1">
+        <f t="array" ref="L85">_xlfn.XLOOKUP(Family[[#This Row],[Mother]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
+        <v>53</v>
+      </c>
+      <c r="M85" t="str" cm="1">
+        <f t="array" ref="M85">_xlfn.XLOOKUP(Family[[#This Row],[Spouse]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
+        <v/>
+      </c>
+      <c r="N85" t="str" cm="1">
+        <f t="array" ref="N85">lambda_lifetimeage(Family[[#This Row],[BirthDate]],Family[[#This Row],[DeathDate]])</f>
+        <v/>
+      </c>
+      <c r="O85" t="str" cm="1">
+        <f t="array" aca="1" ref="O85" ca="1">lambda_currentage(Family[[#This Row],[BirthDate]],Family[[#This Row],[DeathDate]],$B$3)</f>
+        <v>11 years, 7 months, 5 days</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A86" s="9">
+        <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
+        <v>81</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>102</v>
+      </c>
       <c r="C86" s="5"/>
-      <c r="D86" s="5"/>
-      <c r="E86" s="6"/>
-      <c r="F86" s="6"/>
-      <c r="G86" s="5"/>
-      <c r="H86" s="5"/>
-      <c r="I86" s="5"/>
+      <c r="D86" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E86" s="6">
+        <v>44335</v>
+      </c>
+      <c r="F86" s="6">
+        <v>45164</v>
+      </c>
+      <c r="G86" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="H86" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="I86" s="6"/>
       <c r="J86" s="5"/>
-    </row>
-    <row r="87" spans="1:15">
-      <c r="B87" s="5"/>
+      <c r="K86" s="9" cm="1">
+        <f t="array" ref="K86">_xlfn.XLOOKUP(Family[[#This Row],[Father]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
+        <v>52</v>
+      </c>
+      <c r="L86" s="9" cm="1">
+        <f t="array" ref="L86">_xlfn.XLOOKUP(Family[[#This Row],[Mother]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
+        <v>53</v>
+      </c>
+      <c r="M86" s="9" t="str" cm="1">
+        <f t="array" ref="M86">_xlfn.XLOOKUP(Family[[#This Row],[Spouse]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
+        <v/>
+      </c>
+      <c r="N86" s="10" t="str" cm="1">
+        <f t="array" ref="N86">lambda_lifetimeage(Family[[#This Row],[BirthDate]],Family[[#This Row],[DeathDate]])</f>
+        <v>2 years, 3 months, 7 days</v>
+      </c>
+      <c r="O86" s="10" t="str" cm="1">
+        <f t="array" ref="O86">lambda_currentage(Family[[#This Row],[BirthDate]],Family[[#This Row],[DeathDate]],$B$3)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A87" s="9">
+        <f>ROW()-ROW(Family[[#Headers],[PersonID]])</f>
+        <v>82</v>
+      </c>
+      <c r="B87" s="5" t="s">
+        <v>103</v>
+      </c>
       <c r="C87" s="5"/>
-      <c r="D87" s="5"/>
-      <c r="E87" s="6"/>
+      <c r="D87" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E87" s="6">
+        <v>45188</v>
+      </c>
       <c r="F87" s="6"/>
-      <c r="G87" s="5"/>
-      <c r="H87" s="5"/>
-      <c r="I87" s="5"/>
+      <c r="G87" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="H87" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="I87" s="6"/>
       <c r="J87" s="5"/>
-    </row>
-    <row r="88" spans="1:15">
+      <c r="K87" s="9" cm="1">
+        <f t="array" ref="K87">_xlfn.XLOOKUP(Family[[#This Row],[Father]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
+        <v>52</v>
+      </c>
+      <c r="L87" s="9" cm="1">
+        <f t="array" ref="L87">_xlfn.XLOOKUP(Family[[#This Row],[Mother]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
+        <v>53</v>
+      </c>
+      <c r="M87" s="9" t="str" cm="1">
+        <f t="array" ref="M87">_xlfn.XLOOKUP(Family[[#This Row],[Spouse]],Family[[Name]:[Name]],Family[[PersonID]:[PersonID]],"",0)</f>
+        <v/>
+      </c>
+      <c r="N87" s="10" t="str" cm="1">
+        <f t="array" ref="N87">lambda_lifetimeage(Family[[#This Row],[BirthDate]],Family[[#This Row],[DeathDate]])</f>
+        <v/>
+      </c>
+      <c r="O87" s="10" t="str" cm="1">
+        <f t="array" aca="1" ref="O87" ca="1">lambda_currentage(Family[[#This Row],[BirthDate]],Family[[#This Row],[DeathDate]],$B$3)</f>
+        <v>2 years, 4 months, 13 days</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B88" s="5"/>
       <c r="C88" s="5"/>
       <c r="D88" s="5"/>
@@ -4670,7 +4786,7 @@
       <c r="I88" s="5"/>
       <c r="J88" s="5"/>
     </row>
-    <row r="89" spans="1:15">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B89" s="5"/>
       <c r="C89" s="5"/>
       <c r="D89" s="5"/>
@@ -4681,7 +4797,7 @@
       <c r="I89" s="5"/>
       <c r="J89" s="5"/>
     </row>
-    <row r="90" spans="1:15">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B90" s="5"/>
       <c r="C90" s="5"/>
       <c r="D90" s="5"/>
@@ -4692,7 +4808,7 @@
       <c r="I90" s="5"/>
       <c r="J90" s="5"/>
     </row>
-    <row r="91" spans="1:15">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B91" s="5"/>
       <c r="C91" s="5"/>
       <c r="D91" s="5"/>
@@ -4703,7 +4819,7 @@
       <c r="I91" s="5"/>
       <c r="J91" s="5"/>
     </row>
-    <row r="92" spans="1:15">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B92" s="5"/>
       <c r="C92" s="5"/>
       <c r="D92" s="5"/>
@@ -4714,7 +4830,7 @@
       <c r="I92" s="5"/>
       <c r="J92" s="5"/>
     </row>
-    <row r="93" spans="1:15">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B93" s="5"/>
       <c r="C93" s="5"/>
       <c r="D93" s="5"/>
@@ -4725,7 +4841,7 @@
       <c r="I93" s="5"/>
       <c r="J93" s="5"/>
     </row>
-    <row r="94" spans="1:15">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B94" s="5"/>
       <c r="C94" s="5"/>
       <c r="D94" s="5"/>
@@ -4736,7 +4852,7 @@
       <c r="I94" s="5"/>
       <c r="J94" s="5"/>
     </row>
-    <row r="95" spans="1:15">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B95" s="5"/>
       <c r="C95" s="5"/>
       <c r="D95" s="5"/>
@@ -4747,7 +4863,7 @@
       <c r="I95" s="5"/>
       <c r="J95" s="5"/>
     </row>
-    <row r="96" spans="1:15">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B96" s="5"/>
       <c r="C96" s="5"/>
       <c r="D96" s="5"/>
@@ -4758,7 +4874,7 @@
       <c r="I96" s="5"/>
       <c r="J96" s="5"/>
     </row>
-    <row r="97" spans="2:10">
+    <row r="97" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B97" s="5"/>
       <c r="C97" s="5"/>
       <c r="D97" s="5"/>
@@ -4769,7 +4885,7 @@
       <c r="I97" s="5"/>
       <c r="J97" s="5"/>
     </row>
-    <row r="98" spans="2:10">
+    <row r="98" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B98" s="5"/>
       <c r="C98" s="5"/>
       <c r="D98" s="5"/>
@@ -4780,7 +4896,7 @@
       <c r="I98" s="5"/>
       <c r="J98" s="5"/>
     </row>
-    <row r="99" spans="2:10">
+    <row r="99" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B99" s="5"/>
       <c r="C99" s="5"/>
       <c r="D99" s="5"/>
@@ -4791,7 +4907,7 @@
       <c r="I99" s="5"/>
       <c r="J99" s="5"/>
     </row>
-    <row r="100" spans="2:10">
+    <row r="100" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B100" s="5"/>
       <c r="C100" s="5"/>
       <c r="D100" s="5"/>
@@ -4802,7 +4918,7 @@
       <c r="I100" s="5"/>
       <c r="J100" s="5"/>
     </row>
-    <row r="101" spans="2:10">
+    <row r="101" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B101" s="5"/>
       <c r="C101" s="5"/>
       <c r="D101" s="5"/>
@@ -4813,7 +4929,7 @@
       <c r="I101" s="5"/>
       <c r="J101" s="5"/>
     </row>
-    <row r="102" spans="2:10">
+    <row r="102" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B102" s="5"/>
       <c r="C102" s="5"/>
       <c r="D102" s="5"/>
@@ -4824,7 +4940,7 @@
       <c r="I102" s="5"/>
       <c r="J102" s="5"/>
     </row>
-    <row r="103" spans="2:10">
+    <row r="103" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B103" s="5"/>
       <c r="C103" s="5"/>
       <c r="D103" s="5"/>
@@ -4835,7 +4951,7 @@
       <c r="I103" s="5"/>
       <c r="J103" s="5"/>
     </row>
-    <row r="104" spans="2:10">
+    <row r="104" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B104" s="5"/>
       <c r="C104" s="5"/>
       <c r="D104" s="5"/>
@@ -4846,7 +4962,7 @@
       <c r="I104" s="5"/>
       <c r="J104" s="5"/>
     </row>
-    <row r="105" spans="2:10">
+    <row r="105" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B105" s="5"/>
       <c r="C105" s="5"/>
       <c r="D105" s="5"/>
@@ -4857,7 +4973,7 @@
       <c r="I105" s="5"/>
       <c r="J105" s="5"/>
     </row>
-    <row r="106" spans="2:10">
+    <row r="106" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B106" s="5"/>
       <c r="C106" s="5"/>
       <c r="D106" s="5"/>
@@ -4868,7 +4984,7 @@
       <c r="I106" s="5"/>
       <c r="J106" s="5"/>
     </row>
-    <row r="107" spans="2:10">
+    <row r="107" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B107" s="5"/>
       <c r="C107" s="5"/>
       <c r="D107" s="5"/>
@@ -4879,7 +4995,7 @@
       <c r="I107" s="5"/>
       <c r="J107" s="5"/>
     </row>
-    <row r="108" spans="2:10">
+    <row r="108" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B108" s="5"/>
       <c r="C108" s="5"/>
       <c r="D108" s="5"/>
@@ -4890,7 +5006,7 @@
       <c r="I108" s="5"/>
       <c r="J108" s="5"/>
     </row>
-    <row r="109" spans="2:10">
+    <row r="109" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B109" s="5"/>
       <c r="C109" s="5"/>
       <c r="D109" s="5"/>
@@ -4901,7 +5017,7 @@
       <c r="I109" s="5"/>
       <c r="J109" s="5"/>
     </row>
-    <row r="110" spans="2:10">
+    <row r="110" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B110" s="5"/>
       <c r="C110" s="5"/>
       <c r="D110" s="5"/>
@@ -4912,7 +5028,7 @@
       <c r="I110" s="5"/>
       <c r="J110" s="5"/>
     </row>
-    <row r="111" spans="2:10">
+    <row r="111" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B111" s="5"/>
       <c r="C111" s="5"/>
       <c r="D111" s="5"/>
@@ -4923,7 +5039,7 @@
       <c r="I111" s="5"/>
       <c r="J111" s="5"/>
     </row>
-    <row r="112" spans="2:10">
+    <row r="112" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B112" s="5"/>
       <c r="C112" s="5"/>
       <c r="D112" s="5"/>
@@ -4934,7 +5050,7 @@
       <c r="I112" s="5"/>
       <c r="J112" s="5"/>
     </row>
-    <row r="113" spans="2:10">
+    <row r="113" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B113" s="5"/>
       <c r="C113" s="5"/>
       <c r="D113" s="5"/>
@@ -4945,7 +5061,7 @@
       <c r="I113" s="5"/>
       <c r="J113" s="5"/>
     </row>
-    <row r="114" spans="2:10">
+    <row r="114" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B114" s="5"/>
       <c r="C114" s="5"/>
       <c r="D114" s="5"/>
@@ -4956,7 +5072,7 @@
       <c r="I114" s="5"/>
       <c r="J114" s="5"/>
     </row>
-    <row r="115" spans="2:10">
+    <row r="115" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B115" s="5"/>
       <c r="C115" s="5"/>
       <c r="D115" s="5"/>
@@ -4967,7 +5083,7 @@
       <c r="I115" s="5"/>
       <c r="J115" s="5"/>
     </row>
-    <row r="116" spans="2:10">
+    <row r="116" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B116" s="5"/>
       <c r="C116" s="5"/>
       <c r="D116" s="5"/>
@@ -4978,7 +5094,7 @@
       <c r="I116" s="5"/>
       <c r="J116" s="5"/>
     </row>
-    <row r="117" spans="2:10">
+    <row r="117" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B117" s="5"/>
       <c r="C117" s="5"/>
       <c r="D117" s="5"/>
@@ -4989,7 +5105,7 @@
       <c r="I117" s="5"/>
       <c r="J117" s="5"/>
     </row>
-    <row r="118" spans="2:10">
+    <row r="118" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B118" s="5"/>
       <c r="C118" s="5"/>
       <c r="D118" s="5"/>
@@ -5000,7 +5116,7 @@
       <c r="I118" s="5"/>
       <c r="J118" s="5"/>
     </row>
-    <row r="119" spans="2:10">
+    <row r="119" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B119" s="5"/>
       <c r="C119" s="5"/>
       <c r="D119" s="5"/>
@@ -5011,7 +5127,7 @@
       <c r="I119" s="5"/>
       <c r="J119" s="5"/>
     </row>
-    <row r="120" spans="2:10">
+    <row r="120" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B120" s="5"/>
       <c r="C120" s="5"/>
       <c r="D120" s="5"/>
@@ -5022,7 +5138,7 @@
       <c r="I120" s="5"/>
       <c r="J120" s="5"/>
     </row>
-    <row r="121" spans="2:10">
+    <row r="121" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B121" s="5"/>
       <c r="C121" s="5"/>
       <c r="D121" s="5"/>
@@ -5033,7 +5149,7 @@
       <c r="I121" s="5"/>
       <c r="J121" s="5"/>
     </row>
-    <row r="122" spans="2:10">
+    <row r="122" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B122" s="5"/>
       <c r="C122" s="5"/>
       <c r="D122" s="5"/>
@@ -5044,7 +5160,7 @@
       <c r="I122" s="5"/>
       <c r="J122" s="5"/>
     </row>
-    <row r="123" spans="2:10">
+    <row r="123" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B123" s="5"/>
       <c r="C123" s="5"/>
       <c r="D123" s="5"/>
@@ -5055,7 +5171,7 @@
       <c r="I123" s="5"/>
       <c r="J123" s="5"/>
     </row>
-    <row r="124" spans="2:10">
+    <row r="124" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B124" s="5"/>
       <c r="C124" s="5"/>
       <c r="D124" s="5"/>
@@ -5066,7 +5182,7 @@
       <c r="I124" s="5"/>
       <c r="J124" s="5"/>
     </row>
-    <row r="125" spans="2:10">
+    <row r="125" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B125" s="5"/>
       <c r="C125" s="5"/>
       <c r="D125" s="5"/>
@@ -5077,7 +5193,7 @@
       <c r="I125" s="5"/>
       <c r="J125" s="5"/>
     </row>
-    <row r="126" spans="2:10">
+    <row r="126" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B126" s="5"/>
       <c r="C126" s="5"/>
       <c r="D126" s="5"/>
@@ -5088,7 +5204,7 @@
       <c r="I126" s="5"/>
       <c r="J126" s="5"/>
     </row>
-    <row r="127" spans="2:10">
+    <row r="127" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B127" s="5"/>
       <c r="C127" s="5"/>
       <c r="D127" s="5"/>
@@ -5099,7 +5215,7 @@
       <c r="I127" s="5"/>
       <c r="J127" s="5"/>
     </row>
-    <row r="128" spans="2:10">
+    <row r="128" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B128" s="5"/>
       <c r="C128" s="5"/>
       <c r="D128" s="5"/>
@@ -5110,7 +5226,7 @@
       <c r="I128" s="5"/>
       <c r="J128" s="5"/>
     </row>
-    <row r="129" spans="2:10">
+    <row r="129" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B129" s="5"/>
       <c r="C129" s="5"/>
       <c r="D129" s="5"/>
@@ -5121,7 +5237,7 @@
       <c r="I129" s="5"/>
       <c r="J129" s="5"/>
     </row>
-    <row r="130" spans="2:10">
+    <row r="130" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B130" s="5"/>
       <c r="C130" s="5"/>
       <c r="D130" s="5"/>
@@ -5132,7 +5248,7 @@
       <c r="I130" s="5"/>
       <c r="J130" s="5"/>
     </row>
-    <row r="131" spans="2:10">
+    <row r="131" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B131" s="5"/>
       <c r="C131" s="5"/>
       <c r="D131" s="5"/>
@@ -5143,7 +5259,7 @@
       <c r="I131" s="5"/>
       <c r="J131" s="5"/>
     </row>
-    <row r="132" spans="2:10">
+    <row r="132" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B132" s="5"/>
       <c r="C132" s="5"/>
       <c r="D132" s="5"/>
@@ -5154,7 +5270,7 @@
       <c r="I132" s="5"/>
       <c r="J132" s="5"/>
     </row>
-    <row r="133" spans="2:10">
+    <row r="133" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B133" s="5"/>
       <c r="C133" s="5"/>
       <c r="D133" s="5"/>
@@ -5165,7 +5281,7 @@
       <c r="I133" s="5"/>
       <c r="J133" s="5"/>
     </row>
-    <row r="134" spans="2:10">
+    <row r="134" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B134" s="5"/>
       <c r="C134" s="5"/>
       <c r="D134" s="5"/>
@@ -5176,7 +5292,7 @@
       <c r="I134" s="5"/>
       <c r="J134" s="5"/>
     </row>
-    <row r="135" spans="2:10">
+    <row r="135" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B135" s="5"/>
       <c r="C135" s="5"/>
       <c r="D135" s="5"/>
@@ -5187,7 +5303,7 @@
       <c r="I135" s="5"/>
       <c r="J135" s="5"/>
     </row>
-    <row r="136" spans="2:10">
+    <row r="136" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B136" s="5"/>
       <c r="C136" s="5"/>
       <c r="D136" s="5"/>
@@ -5198,7 +5314,7 @@
       <c r="I136" s="5"/>
       <c r="J136" s="5"/>
     </row>
-    <row r="137" spans="2:10">
+    <row r="137" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B137" s="5"/>
       <c r="C137" s="5"/>
       <c r="D137" s="5"/>
@@ -5209,7 +5325,7 @@
       <c r="I137" s="5"/>
       <c r="J137" s="5"/>
     </row>
-    <row r="138" spans="2:10">
+    <row r="138" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B138" s="5"/>
       <c r="C138" s="5"/>
       <c r="D138" s="5"/>
@@ -5220,7 +5336,7 @@
       <c r="I138" s="5"/>
       <c r="J138" s="5"/>
     </row>
-    <row r="139" spans="2:10">
+    <row r="139" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B139" s="5"/>
       <c r="C139" s="5"/>
       <c r="D139" s="5"/>
@@ -5231,7 +5347,7 @@
       <c r="I139" s="5"/>
       <c r="J139" s="5"/>
     </row>
-    <row r="140" spans="2:10">
+    <row r="140" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B140" s="5"/>
       <c r="C140" s="5"/>
       <c r="D140" s="5"/>
@@ -5242,7 +5358,7 @@
       <c r="I140" s="5"/>
       <c r="J140" s="5"/>
     </row>
-    <row r="141" spans="2:10">
+    <row r="141" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B141" s="5"/>
       <c r="C141" s="5"/>
       <c r="D141" s="5"/>
@@ -5253,7 +5369,7 @@
       <c r="I141" s="5"/>
       <c r="J141" s="5"/>
     </row>
-    <row r="142" spans="2:10">
+    <row r="142" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B142" s="5"/>
       <c r="C142" s="5"/>
       <c r="D142" s="5"/>
@@ -5264,7 +5380,7 @@
       <c r="I142" s="5"/>
       <c r="J142" s="5"/>
     </row>
-    <row r="143" spans="2:10">
+    <row r="143" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B143" s="5"/>
       <c r="C143" s="5"/>
       <c r="D143" s="5"/>
@@ -5275,7 +5391,7 @@
       <c r="I143" s="5"/>
       <c r="J143" s="5"/>
     </row>
-    <row r="144" spans="2:10">
+    <row r="144" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B144" s="5"/>
       <c r="C144" s="5"/>
       <c r="D144" s="5"/>
@@ -5286,7 +5402,7 @@
       <c r="I144" s="5"/>
       <c r="J144" s="5"/>
     </row>
-    <row r="145" spans="2:10">
+    <row r="145" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B145" s="5"/>
       <c r="C145" s="5"/>
       <c r="D145" s="5"/>
@@ -5297,7 +5413,7 @@
       <c r="I145" s="5"/>
       <c r="J145" s="5"/>
     </row>
-    <row r="146" spans="2:10">
+    <row r="146" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B146" s="5"/>
       <c r="C146" s="5"/>
       <c r="D146" s="5"/>
@@ -5308,7 +5424,7 @@
       <c r="I146" s="5"/>
       <c r="J146" s="5"/>
     </row>
-    <row r="147" spans="2:10">
+    <row r="147" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B147" s="5"/>
       <c r="C147" s="5"/>
       <c r="D147" s="5"/>
@@ -5319,7 +5435,7 @@
       <c r="I147" s="5"/>
       <c r="J147" s="5"/>
     </row>
-    <row r="148" spans="2:10">
+    <row r="148" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B148" s="5"/>
       <c r="C148" s="5"/>
       <c r="D148" s="5"/>
@@ -5330,7 +5446,7 @@
       <c r="I148" s="5"/>
       <c r="J148" s="5"/>
     </row>
-    <row r="149" spans="2:10">
+    <row r="149" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B149" s="5"/>
       <c r="C149" s="5"/>
       <c r="D149" s="5"/>
@@ -5341,7 +5457,7 @@
       <c r="I149" s="5"/>
       <c r="J149" s="5"/>
     </row>
-    <row r="150" spans="2:10">
+    <row r="150" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B150" s="5"/>
       <c r="C150" s="5"/>
       <c r="D150" s="5"/>
@@ -5352,7 +5468,7 @@
       <c r="I150" s="5"/>
       <c r="J150" s="5"/>
     </row>
-    <row r="151" spans="2:10">
+    <row r="151" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B151" s="5"/>
       <c r="C151" s="5"/>
       <c r="D151" s="5"/>
@@ -5363,7 +5479,7 @@
       <c r="I151" s="5"/>
       <c r="J151" s="5"/>
     </row>
-    <row r="152" spans="2:10">
+    <row r="152" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B152" s="5"/>
       <c r="C152" s="5"/>
       <c r="D152" s="5"/>
@@ -5374,7 +5490,7 @@
       <c r="I152" s="5"/>
       <c r="J152" s="5"/>
     </row>
-    <row r="153" spans="2:10">
+    <row r="153" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B153" s="5"/>
       <c r="C153" s="5"/>
       <c r="D153" s="5"/>
@@ -5385,7 +5501,7 @@
       <c r="I153" s="5"/>
       <c r="J153" s="5"/>
     </row>
-    <row r="154" spans="2:10">
+    <row r="154" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B154" s="5"/>
       <c r="C154" s="5"/>
       <c r="D154" s="5"/>
@@ -5396,7 +5512,7 @@
       <c r="I154" s="5"/>
       <c r="J154" s="5"/>
     </row>
-    <row r="155" spans="2:10">
+    <row r="155" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B155" s="5"/>
       <c r="C155" s="5"/>
       <c r="D155" s="5"/>
@@ -5407,7 +5523,7 @@
       <c r="I155" s="5"/>
       <c r="J155" s="5"/>
     </row>
-    <row r="156" spans="2:10">
+    <row r="156" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B156" s="5"/>
       <c r="C156" s="5"/>
       <c r="D156" s="5"/>
@@ -5418,7 +5534,7 @@
       <c r="I156" s="5"/>
       <c r="J156" s="5"/>
     </row>
-    <row r="157" spans="2:10">
+    <row r="157" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B157" s="5"/>
       <c r="C157" s="5"/>
       <c r="D157" s="5"/>
@@ -5429,7 +5545,7 @@
       <c r="I157" s="5"/>
       <c r="J157" s="5"/>
     </row>
-    <row r="158" spans="2:10">
+    <row r="158" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B158" s="5"/>
       <c r="C158" s="5"/>
       <c r="D158" s="5"/>
@@ -5440,7 +5556,7 @@
       <c r="I158" s="5"/>
       <c r="J158" s="5"/>
     </row>
-    <row r="159" spans="2:10">
+    <row r="159" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B159" s="5"/>
       <c r="C159" s="5"/>
       <c r="D159" s="5"/>
@@ -5451,7 +5567,7 @@
       <c r="I159" s="5"/>
       <c r="J159" s="5"/>
     </row>
-    <row r="160" spans="2:10">
+    <row r="160" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B160" s="5"/>
       <c r="C160" s="5"/>
       <c r="D160" s="5"/>
@@ -5462,7 +5578,7 @@
       <c r="I160" s="5"/>
       <c r="J160" s="5"/>
     </row>
-    <row r="161" spans="2:10">
+    <row r="161" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B161" s="5"/>
       <c r="C161" s="5"/>
       <c r="D161" s="5"/>
@@ -5473,7 +5589,7 @@
       <c r="I161" s="5"/>
       <c r="J161" s="5"/>
     </row>
-    <row r="162" spans="2:10">
+    <row r="162" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B162" s="5"/>
       <c r="C162" s="5"/>
       <c r="D162" s="5"/>
@@ -5484,7 +5600,7 @@
       <c r="I162" s="5"/>
       <c r="J162" s="5"/>
     </row>
-    <row r="163" spans="2:10">
+    <row r="163" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B163" s="5"/>
       <c r="C163" s="5"/>
       <c r="D163" s="5"/>
@@ -5495,7 +5611,7 @@
       <c r="I163" s="5"/>
       <c r="J163" s="5"/>
     </row>
-    <row r="164" spans="2:10">
+    <row r="164" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B164" s="5"/>
       <c r="C164" s="5"/>
       <c r="D164" s="5"/>
@@ -5506,7 +5622,7 @@
       <c r="I164" s="5"/>
       <c r="J164" s="5"/>
     </row>
-    <row r="165" spans="2:10">
+    <row r="165" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B165" s="5"/>
       <c r="C165" s="5"/>
       <c r="D165" s="5"/>
@@ -5517,7 +5633,7 @@
       <c r="I165" s="5"/>
       <c r="J165" s="5"/>
     </row>
-    <row r="166" spans="2:10">
+    <row r="166" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B166" s="5"/>
       <c r="C166" s="5"/>
       <c r="D166" s="5"/>
@@ -5528,7 +5644,7 @@
       <c r="I166" s="5"/>
       <c r="J166" s="5"/>
     </row>
-    <row r="167" spans="2:10">
+    <row r="167" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B167" s="5"/>
       <c r="C167" s="5"/>
       <c r="D167" s="5"/>
@@ -5539,7 +5655,7 @@
       <c r="I167" s="5"/>
       <c r="J167" s="5"/>
     </row>
-    <row r="168" spans="2:10">
+    <row r="168" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B168" s="5"/>
       <c r="C168" s="5"/>
       <c r="D168" s="5"/>
@@ -5550,7 +5666,7 @@
       <c r="I168" s="5"/>
       <c r="J168" s="5"/>
     </row>
-    <row r="169" spans="2:10">
+    <row r="169" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B169" s="5"/>
       <c r="C169" s="5"/>
       <c r="D169" s="5"/>
@@ -5561,7 +5677,7 @@
       <c r="I169" s="5"/>
       <c r="J169" s="5"/>
     </row>
-    <row r="170" spans="2:10">
+    <row r="170" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B170" s="5"/>
       <c r="C170" s="5"/>
       <c r="D170" s="5"/>
@@ -5572,7 +5688,7 @@
       <c r="I170" s="5"/>
       <c r="J170" s="5"/>
     </row>
-    <row r="171" spans="2:10">
+    <row r="171" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B171" s="5"/>
       <c r="C171" s="5"/>
       <c r="D171" s="5"/>
@@ -5583,7 +5699,7 @@
       <c r="I171" s="5"/>
       <c r="J171" s="5"/>
     </row>
-    <row r="172" spans="2:10">
+    <row r="172" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B172" s="5"/>
       <c r="C172" s="5"/>
       <c r="D172" s="5"/>
@@ -5594,7 +5710,7 @@
       <c r="I172" s="5"/>
       <c r="J172" s="5"/>
     </row>
-    <row r="173" spans="2:10">
+    <row r="173" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B173" s="5"/>
       <c r="C173" s="5"/>
       <c r="D173" s="5"/>
@@ -5605,7 +5721,7 @@
       <c r="I173" s="5"/>
       <c r="J173" s="5"/>
     </row>
-    <row r="174" spans="2:10">
+    <row r="174" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B174" s="5"/>
       <c r="C174" s="5"/>
       <c r="D174" s="5"/>
@@ -5616,7 +5732,7 @@
       <c r="I174" s="5"/>
       <c r="J174" s="5"/>
     </row>
-    <row r="175" spans="2:10">
+    <row r="175" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B175" s="5"/>
       <c r="C175" s="5"/>
       <c r="D175" s="5"/>
@@ -5627,7 +5743,7 @@
       <c r="I175" s="5"/>
       <c r="J175" s="5"/>
     </row>
-    <row r="176" spans="2:10">
+    <row r="176" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B176" s="5"/>
       <c r="C176" s="5"/>
       <c r="D176" s="5"/>
@@ -5638,7 +5754,7 @@
       <c r="I176" s="5"/>
       <c r="J176" s="5"/>
     </row>
-    <row r="177" spans="2:10">
+    <row r="177" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B177" s="5"/>
       <c r="C177" s="5"/>
       <c r="D177" s="5"/>
@@ -5649,7 +5765,7 @@
       <c r="I177" s="5"/>
       <c r="J177" s="5"/>
     </row>
-    <row r="178" spans="2:10">
+    <row r="178" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B178" s="5"/>
       <c r="C178" s="5"/>
       <c r="D178" s="5"/>
@@ -5660,7 +5776,7 @@
       <c r="I178" s="5"/>
       <c r="J178" s="5"/>
     </row>
-    <row r="179" spans="2:10">
+    <row r="179" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B179" s="5"/>
       <c r="C179" s="5"/>
       <c r="D179" s="5"/>
@@ -5671,7 +5787,7 @@
       <c r="I179" s="5"/>
       <c r="J179" s="5"/>
     </row>
-    <row r="180" spans="2:10">
+    <row r="180" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B180" s="5"/>
       <c r="C180" s="5"/>
       <c r="D180" s="5"/>
@@ -5682,7 +5798,7 @@
       <c r="I180" s="5"/>
       <c r="J180" s="5"/>
     </row>
-    <row r="181" spans="2:10">
+    <row r="181" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B181" s="5"/>
       <c r="C181" s="5"/>
       <c r="D181" s="5"/>
@@ -5693,7 +5809,7 @@
       <c r="I181" s="5"/>
       <c r="J181" s="5"/>
     </row>
-    <row r="182" spans="2:10">
+    <row r="182" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B182" s="5"/>
       <c r="C182" s="5"/>
       <c r="D182" s="5"/>
@@ -5704,7 +5820,7 @@
       <c r="I182" s="5"/>
       <c r="J182" s="5"/>
     </row>
-    <row r="183" spans="2:10">
+    <row r="183" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B183" s="5"/>
       <c r="C183" s="5"/>
       <c r="D183" s="5"/>
@@ -5715,7 +5831,7 @@
       <c r="I183" s="5"/>
       <c r="J183" s="5"/>
     </row>
-    <row r="184" spans="2:10">
+    <row r="184" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B184" s="5"/>
       <c r="C184" s="5"/>
       <c r="D184" s="5"/>
@@ -5726,7 +5842,7 @@
       <c r="I184" s="5"/>
       <c r="J184" s="5"/>
     </row>
-    <row r="185" spans="2:10">
+    <row r="185" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B185" s="5"/>
       <c r="C185" s="5"/>
       <c r="D185" s="5"/>
@@ -5737,7 +5853,7 @@
       <c r="I185" s="5"/>
       <c r="J185" s="5"/>
     </row>
-    <row r="186" spans="2:10">
+    <row r="186" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B186" s="5"/>
       <c r="C186" s="5"/>
       <c r="D186" s="5"/>
@@ -5748,7 +5864,7 @@
       <c r="I186" s="5"/>
       <c r="J186" s="5"/>
     </row>
-    <row r="187" spans="2:10">
+    <row r="187" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B187" s="5"/>
       <c r="C187" s="5"/>
       <c r="D187" s="5"/>
@@ -5759,7 +5875,7 @@
       <c r="I187" s="5"/>
       <c r="J187" s="5"/>
     </row>
-    <row r="188" spans="2:10">
+    <row r="188" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B188" s="5"/>
       <c r="C188" s="5"/>
       <c r="D188" s="5"/>
@@ -5770,7 +5886,7 @@
       <c r="I188" s="5"/>
       <c r="J188" s="5"/>
     </row>
-    <row r="189" spans="2:10">
+    <row r="189" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B189" s="5"/>
       <c r="C189" s="5"/>
       <c r="D189" s="5"/>
@@ -5781,7 +5897,7 @@
       <c r="I189" s="5"/>
       <c r="J189" s="5"/>
     </row>
-    <row r="190" spans="2:10">
+    <row r="190" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B190" s="5"/>
       <c r="C190" s="5"/>
       <c r="D190" s="5"/>
@@ -5792,7 +5908,7 @@
       <c r="I190" s="5"/>
       <c r="J190" s="5"/>
     </row>
-    <row r="191" spans="2:10">
+    <row r="191" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B191" s="5"/>
       <c r="C191" s="5"/>
       <c r="D191" s="5"/>
@@ -5803,7 +5919,7 @@
       <c r="I191" s="5"/>
       <c r="J191" s="5"/>
     </row>
-    <row r="192" spans="2:10">
+    <row r="192" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B192" s="5"/>
       <c r="C192" s="5"/>
       <c r="D192" s="5"/>
@@ -5814,7 +5930,7 @@
       <c r="I192" s="5"/>
       <c r="J192" s="5"/>
     </row>
-    <row r="193" spans="2:10">
+    <row r="193" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B193" s="5"/>
       <c r="C193" s="5"/>
       <c r="D193" s="5"/>
@@ -5825,7 +5941,7 @@
       <c r="I193" s="5"/>
       <c r="J193" s="5"/>
     </row>
-    <row r="194" spans="2:10">
+    <row r="194" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B194" s="5"/>
       <c r="C194" s="5"/>
       <c r="D194" s="5"/>
@@ -5836,7 +5952,7 @@
       <c r="I194" s="5"/>
       <c r="J194" s="5"/>
     </row>
-    <row r="195" spans="2:10">
+    <row r="195" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B195" s="5"/>
       <c r="C195" s="5"/>
       <c r="D195" s="5"/>
@@ -5847,7 +5963,7 @@
       <c r="I195" s="5"/>
       <c r="J195" s="5"/>
     </row>
-    <row r="196" spans="2:10">
+    <row r="196" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B196" s="5"/>
       <c r="C196" s="5"/>
       <c r="D196" s="5"/>
@@ -5858,7 +5974,7 @@
       <c r="I196" s="5"/>
       <c r="J196" s="5"/>
     </row>
-    <row r="197" spans="2:10">
+    <row r="197" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B197" s="5"/>
       <c r="C197" s="5"/>
       <c r="D197" s="5"/>
@@ -5869,7 +5985,7 @@
       <c r="I197" s="5"/>
       <c r="J197" s="5"/>
     </row>
-    <row r="198" spans="2:10">
+    <row r="198" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B198" s="5"/>
       <c r="C198" s="5"/>
       <c r="D198" s="5"/>
@@ -5880,7 +5996,7 @@
       <c r="I198" s="5"/>
       <c r="J198" s="5"/>
     </row>
-    <row r="199" spans="2:10">
+    <row r="199" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B199" s="5"/>
       <c r="C199" s="5"/>
       <c r="D199" s="5"/>
@@ -5891,7 +6007,7 @@
       <c r="I199" s="5"/>
       <c r="J199" s="5"/>
     </row>
-    <row r="200" spans="2:10">
+    <row r="200" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B200" s="5"/>
       <c r="C200" s="5"/>
       <c r="D200" s="5"/>
@@ -5902,7 +6018,7 @@
       <c r="I200" s="5"/>
       <c r="J200" s="5"/>
     </row>
-    <row r="201" spans="2:10">
+    <row r="201" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B201" s="5"/>
       <c r="C201" s="5"/>
       <c r="D201" s="5"/>
@@ -5913,7 +6029,7 @@
       <c r="I201" s="5"/>
       <c r="J201" s="5"/>
     </row>
-    <row r="202" spans="2:10">
+    <row r="202" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B202" s="5"/>
       <c r="C202" s="5"/>
       <c r="D202" s="5"/>
@@ -5924,7 +6040,7 @@
       <c r="I202" s="5"/>
       <c r="J202" s="5"/>
     </row>
-    <row r="203" spans="2:10">
+    <row r="203" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B203" s="5"/>
       <c r="C203" s="5"/>
       <c r="D203" s="5"/>
@@ -5935,7 +6051,7 @@
       <c r="I203" s="5"/>
       <c r="J203" s="5"/>
     </row>
-    <row r="204" spans="2:10">
+    <row r="204" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B204" s="5"/>
       <c r="C204" s="5"/>
       <c r="D204" s="5"/>
@@ -5946,7 +6062,7 @@
       <c r="I204" s="5"/>
       <c r="J204" s="5"/>
     </row>
-    <row r="205" spans="2:10">
+    <row r="205" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B205" s="5"/>
       <c r="C205" s="5"/>
       <c r="D205" s="5"/>
@@ -5957,20 +6073,31 @@
       <c r="I205" s="5"/>
       <c r="J205" s="5"/>
     </row>
+    <row r="206" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B206" s="5"/>
+      <c r="C206" s="5"/>
+      <c r="D206" s="5"/>
+      <c r="E206" s="6"/>
+      <c r="F206" s="6"/>
+      <c r="G206" s="5"/>
+      <c r="H206" s="5"/>
+      <c r="I206" s="5"/>
+      <c r="J206" s="5"/>
+    </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="OSXJL2j2klc/3rV8JR0C05heaM4HFLFyBsFnOWmv6JuJKXv3Z8lH92zSsabSI5cV9dHuaC6y4rg1Y2KlTOEjXA==" saltValue="voqt7IrGQpq392JNuj33JQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="8tElWfJnWP+A652nkbOenVe0TIPHMqB+hzMn2S0e/Qf6R6AzhLYCgGtJw73kwlXibS6hWKY2e11QLr8oc0H1NA==" saltValue="MErHZgUwbc9mlqPOljtERQ==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D59:D84 D6:D58" xr:uid="{88B235F2-0B48-45BB-976F-4DE8389AF51E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:D85" xr:uid="{88B235F2-0B48-45BB-976F-4DE8389AF51E}">
       <formula1>INDIRECT("Lookup_Gender[Gender]")</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G59:J84 G6:J58" xr:uid="{22E5EF5B-D42A-4822-8EC6-9949242216BD}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:J85" xr:uid="{22E5EF5B-D42A-4822-8EC6-9949242216BD}">
       <formula1>INDIRECT("Family[name]")</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="G6:I16 I18:I22 I24:I51 I58 I53:I56 I59:I84 G59:H84 G53:H56 G58:H58 G24:H51 G18:H22 G17:H17 G23:H23 G52:H52 G57:H57" listDataValidation="1"/>
+    <ignoredError sqref="G6:I16 I18:I22 I24:I51 I58 I53:I56 I63:I85 G63:H85 G53:H56 G58:H58 G24:H51 G18:H22 G17:H17 G23:H23 G52:H52 G57:H57 G59:H61 I59:I60" listDataValidation="1"/>
   </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
@@ -5983,28 +6110,28 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A5:L84"/>
+  <dimension ref="A5:L87"/>
   <sheetViews>
     <sheetView showGridLines="0" showZeros="0" workbookViewId="0">
       <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
@@ -6042,57 +6169,57 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" cm="1">
-        <f t="array" ref="A6:A84">Family[PersonID]</f>
+        <f t="array" ref="A6:A87">Family[PersonID]</f>
         <v>1</v>
       </c>
       <c r="B6" t="str" cm="1">
-        <f t="array" ref="B6:B84">_xlfn.XLOOKUP(_xlfn.ANCHORARRAY($A$6),Family[[PersonID]:[PersonID]],Family[Name],"",0)</f>
+        <f t="array" ref="B6:B87">_xlfn.XLOOKUP(_xlfn.ANCHORARRAY($A$6),Family[[PersonID]:[PersonID]],Family[Name],"",0)</f>
         <v>Jose G. Alto</v>
       </c>
       <c r="C6" cm="1">
-        <f t="array" ref="C6:C84">_xlfn.XLOOKUP(_xlfn.ANCHORARRAY($A$6),Family[[PersonID]:[PersonID]],Family[Nickname],"",0)</f>
+        <f t="array" ref="C6:C87">_xlfn.XLOOKUP(_xlfn.ANCHORARRAY($A$6),Family[[PersonID]:[PersonID]],Family[Nickname],"",0)</f>
         <v>0</v>
       </c>
       <c r="D6" t="str" cm="1">
-        <f t="array" ref="D6:D84">_xlfn.XLOOKUP(_xlfn.ANCHORARRAY($A$6),Family[[PersonID]:[PersonID]],Family[Gender],"",0)</f>
+        <f t="array" ref="D6:D87">_xlfn.XLOOKUP(_xlfn.ANCHORARRAY($A$6),Family[[PersonID]:[PersonID]],Family[Gender],"",0)</f>
         <v>male</v>
       </c>
       <c r="E6" s="3" cm="1">
-        <f t="array" ref="E6:E84">_xlfn.XLOOKUP(_xlfn.ANCHORARRAY($A$6),Family[[PersonID]:[PersonID]],Family[BirthDate],"",0)</f>
+        <f t="array" ref="E6:E87">_xlfn.XLOOKUP(_xlfn.ANCHORARRAY($A$6),Family[[PersonID]:[PersonID]],Family[BirthDate],"",0)</f>
         <v>1174</v>
       </c>
       <c r="F6" s="3" cm="1">
-        <f t="array" ref="F6:F84">_xlfn.XLOOKUP(_xlfn.ANCHORARRAY($A$6),Family[[PersonID]:[PersonID]],Family[DeathDate],"",0)</f>
+        <f t="array" ref="F6:F87">_xlfn.XLOOKUP(_xlfn.ANCHORARRAY($A$6),Family[[PersonID]:[PersonID]],Family[DeathDate],"",0)</f>
         <v>32314</v>
       </c>
       <c r="G6" t="str" cm="1">
-        <f t="array" ref="G6:G84">_xlfn.XLOOKUP(_xlfn.ANCHORARRAY($A$6),Family[[PersonID]:[PersonID]],Family[FatherID],"",0)</f>
+        <f t="array" ref="G6:G87">_xlfn.XLOOKUP(_xlfn.ANCHORARRAY($A$6),Family[[PersonID]:[PersonID]],Family[FatherID],"",0)</f>
         <v/>
       </c>
       <c r="H6" t="str" cm="1">
-        <f t="array" ref="H6:H84">_xlfn.XLOOKUP(_xlfn.ANCHORARRAY($A$6),Family[[PersonID]:[PersonID]],Family[MotherID],"",0)</f>
+        <f t="array" ref="H6:H87">_xlfn.XLOOKUP(_xlfn.ANCHORARRAY($A$6),Family[[PersonID]:[PersonID]],Family[MotherID],"",0)</f>
         <v/>
       </c>
       <c r="I6" cm="1">
-        <f t="array" ref="I6:I84">_xlfn.XLOOKUP(_xlfn.ANCHORARRAY($A$6),Family[[PersonID]:[PersonID]],Family[SpouseID],"",0)</f>
+        <f t="array" ref="I6:I87">_xlfn.XLOOKUP(_xlfn.ANCHORARRAY($A$6),Family[[PersonID]:[PersonID]],Family[SpouseID],"",0)</f>
         <v>2</v>
       </c>
       <c r="J6" t="str" cm="1">
-        <f t="array" ref="J6:J84">_xlfn.XLOOKUP(_xlfn.ANCHORARRAY($A$6),Family[[PersonID]:[PersonID]],Family[LifeTime Age],"",0)</f>
+        <f t="array" ref="J6:J87">_xlfn.XLOOKUP(_xlfn.ANCHORARRAY($A$6),Family[[PersonID]:[PersonID]],Family[LifeTime Age],"",0)</f>
         <v>85 years, 3 months, 1 days</v>
       </c>
       <c r="K6" t="str" cm="1">
-        <f t="array" aca="1" ref="K6:K84" ca="1">_xlfn.XLOOKUP(_xlfn.ANCHORARRAY($A$6),Family[[PersonID]:[PersonID]],Family[Current Age],"",0)</f>
+        <f t="array" aca="1" ref="K6:K87" ca="1">_xlfn.XLOOKUP(_xlfn.ANCHORARRAY($A$6),Family[[PersonID]:[PersonID]],Family[Current Age],"",0)</f>
         <v/>
       </c>
       <c r="L6" cm="1">
-        <f t="array" ref="L6:L84">_xlfn.XLOOKUP(_xlfn.ANCHORARRAY($A$6),Family[[PersonID]:[PersonID]],Family[Notes],"",0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+        <f t="array" ref="L6:L87">_xlfn.XLOOKUP(_xlfn.ANCHORARRAY($A$6),Family[[PersonID]:[PersonID]],Family[Notes],"",0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2</v>
       </c>
@@ -6131,7 +6258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>3</v>
       </c>
@@ -6170,7 +6297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>4</v>
       </c>
@@ -6203,13 +6330,13 @@
       </c>
       <c r="K9" t="str">
         <f ca="1"/>
-        <v>92 years, 1 months, 23 days</v>
+        <v>92 years, 1 months, 25 days</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>5</v>
       </c>
@@ -6248,7 +6375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>6</v>
       </c>
@@ -6281,13 +6408,13 @@
       </c>
       <c r="K11" t="str">
         <f ca="1"/>
-        <v>90 years, 0 months, 17 days</v>
+        <v>90 years, 0 months, 19 days</v>
       </c>
       <c r="L11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>7</v>
       </c>
@@ -6326,7 +6453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>8</v>
       </c>
@@ -6359,13 +6486,13 @@
       </c>
       <c r="K13" t="str">
         <f ca="1"/>
-        <v>85 years, 7 months, 10 days</v>
+        <v>85 years, 7 months, 12 days</v>
       </c>
       <c r="L13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>9</v>
       </c>
@@ -6404,7 +6531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>10</v>
       </c>
@@ -6437,13 +6564,13 @@
       </c>
       <c r="K15" t="str">
         <f ca="1"/>
-        <v>83 years, 6 months, 29 days</v>
+        <v>83 years, 7 months, 0 days</v>
       </c>
       <c r="L15">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>11</v>
       </c>
@@ -6482,7 +6609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>12</v>
       </c>
@@ -6521,7 +6648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>13</v>
       </c>
@@ -6554,13 +6681,13 @@
       </c>
       <c r="K18" t="str">
         <f ca="1"/>
-        <v>78 years, 1 months, 24 days</v>
+        <v>78 years, 1 months, 26 days</v>
       </c>
       <c r="L18">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>14</v>
       </c>
@@ -6599,7 +6726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>15</v>
       </c>
@@ -6638,7 +6765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>16</v>
       </c>
@@ -6671,13 +6798,13 @@
       </c>
       <c r="K21" t="str">
         <f ca="1"/>
-        <v>71 years, 10 months, 15 days</v>
+        <v>71 years, 10 months, 17 days</v>
       </c>
       <c r="L21">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>17</v>
       </c>
@@ -6716,7 +6843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>18</v>
       </c>
@@ -6755,7 +6882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>19</v>
       </c>
@@ -6788,13 +6915,13 @@
       </c>
       <c r="K24" t="str">
         <f ca="1"/>
-        <v>69 years, 4 months, 16 days</v>
+        <v>69 years, 4 months, 18 days</v>
       </c>
       <c r="L24">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>20</v>
       </c>
@@ -6833,7 +6960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>21</v>
       </c>
@@ -6872,7 +6999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>22</v>
       </c>
@@ -6911,7 +7038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>23</v>
       </c>
@@ -6950,7 +7077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>24</v>
       </c>
@@ -6989,7 +7116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>25</v>
       </c>
@@ -7028,7 +7155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>26</v>
       </c>
@@ -7067,7 +7194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>27</v>
       </c>
@@ -7106,7 +7233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>28</v>
       </c>
@@ -7145,7 +7272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>29</v>
       </c>
@@ -7184,7 +7311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>30</v>
       </c>
@@ -7223,7 +7350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>31</v>
       </c>
@@ -7262,7 +7389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>32</v>
       </c>
@@ -7301,7 +7428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>33</v>
       </c>
@@ -7340,7 +7467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>34</v>
       </c>
@@ -7379,7 +7506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>35</v>
       </c>
@@ -7418,7 +7545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>36</v>
       </c>
@@ -7457,7 +7584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>37</v>
       </c>
@@ -7496,7 +7623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>38</v>
       </c>
@@ -7535,7 +7662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:12">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>39</v>
       </c>
@@ -7574,7 +7701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>40</v>
       </c>
@@ -7613,7 +7740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:12">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>41</v>
       </c>
@@ -7652,7 +7779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:12">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>42</v>
       </c>
@@ -7691,7 +7818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:12">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>43</v>
       </c>
@@ -7730,7 +7857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:12">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>44</v>
       </c>
@@ -7769,7 +7896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:12">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>45</v>
       </c>
@@ -7808,7 +7935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:12">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>46</v>
       </c>
@@ -7847,7 +7974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:12">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>47</v>
       </c>
@@ -7886,7 +8013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:12">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>48</v>
       </c>
@@ -7925,7 +8052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:12">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>49</v>
       </c>
@@ -7964,7 +8091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:12">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>50</v>
       </c>
@@ -8003,7 +8130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:12">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>51</v>
       </c>
@@ -8042,7 +8169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:12">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>52</v>
       </c>
@@ -8081,7 +8208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:12">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>53</v>
       </c>
@@ -8120,7 +8247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:12">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>54</v>
       </c>
@@ -8159,7 +8286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:12">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>55</v>
       </c>
@@ -8198,7 +8325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:12">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>56</v>
       </c>
@@ -8223,8 +8350,8 @@
       <c r="H61">
         <v>19</v>
       </c>
-      <c r="I61" t="str">
-        <v/>
+      <c r="I61">
+        <v>57</v>
       </c>
       <c r="J61" t="str">
         <v/>
@@ -8237,12 +8364,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:12">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>57</v>
       </c>
       <c r="B62" t="str">
-        <v>Julie Wongbandue</v>
+        <v>Nita Nash Wongbandue</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -8256,14 +8383,14 @@
       <c r="F62" s="3">
         <v>0</v>
       </c>
-      <c r="G62">
-        <v>18</v>
-      </c>
-      <c r="H62">
-        <v>19</v>
-      </c>
-      <c r="I62" t="str">
-        <v/>
+      <c r="G62" t="str">
+        <v/>
+      </c>
+      <c r="H62" t="str">
+        <v/>
+      </c>
+      <c r="I62">
+        <v>56</v>
       </c>
       <c r="J62" t="str">
         <v/>
@@ -8276,12 +8403,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:12">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>58</v>
       </c>
       <c r="B63" t="str">
-        <v>Denice Alto</v>
+        <v>Julie Wongbandue</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -8296,10 +8423,10 @@
         <v>0</v>
       </c>
       <c r="G63">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H63">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I63" t="str">
         <v/>
@@ -8315,18 +8442,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:12">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>59</v>
       </c>
       <c r="B64" t="str">
-        <v>Nicolas Miles Alto</v>
+        <v>Denice Alto</v>
       </c>
       <c r="C64">
         <v>0</v>
       </c>
       <c r="D64" t="str">
-        <v>male</v>
+        <v>female</v>
       </c>
       <c r="E64" s="3">
         <v>0</v>
@@ -8354,18 +8481,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:12">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>60</v>
       </c>
       <c r="B65" t="str">
-        <v>Ava Margaux Alto</v>
+        <v>Nicolas Miles Alto</v>
       </c>
       <c r="C65">
         <v>0</v>
       </c>
       <c r="D65" t="str">
-        <v>female</v>
+        <v>male</v>
       </c>
       <c r="E65" s="3">
         <v>0</v>
@@ -8374,10 +8501,10 @@
         <v>0</v>
       </c>
       <c r="G65">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H65">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I65" t="str">
         <v/>
@@ -8393,12 +8520,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:12">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>61</v>
       </c>
       <c r="B66" t="str">
-        <v xml:space="preserve">Tifanny Claire </v>
+        <v>Ava Margaux Alto</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -8413,10 +8540,10 @@
         <v>0</v>
       </c>
       <c r="G66">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H66">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I66" t="str">
         <v/>
@@ -8432,18 +8559,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:12">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>62</v>
       </c>
       <c r="B67" t="str">
-        <v>Matthew Ira James</v>
+        <v xml:space="preserve">Tifanny Claire </v>
       </c>
       <c r="C67">
         <v>0</v>
       </c>
       <c r="D67" t="str">
-        <v>male</v>
+        <v>female</v>
       </c>
       <c r="E67" s="3">
         <v>0</v>
@@ -8471,12 +8598,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:12">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>63</v>
       </c>
       <c r="B68" t="str">
-        <v>Brandon Alto</v>
+        <v>Matthew Ira James</v>
       </c>
       <c r="C68">
         <v>0</v>
@@ -8491,10 +8618,10 @@
         <v>0</v>
       </c>
       <c r="G68">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H68">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I68" t="str">
         <v/>
@@ -8510,12 +8637,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:12">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>64</v>
       </c>
       <c r="B69" t="str">
-        <v>Harold Wilson Alto</v>
+        <v>Brandon Alto</v>
       </c>
       <c r="C69">
         <v>0</v>
@@ -8530,10 +8657,10 @@
         <v>0</v>
       </c>
       <c r="G69">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H69">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I69" t="str">
         <v/>
@@ -8549,18 +8676,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:12">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>65</v>
       </c>
       <c r="B70" t="str">
-        <v>Sophia Joy Alto</v>
+        <v>Harold Wilson Alto</v>
       </c>
       <c r="C70">
         <v>0</v>
       </c>
       <c r="D70" t="str">
-        <v>female</v>
+        <v>male</v>
       </c>
       <c r="E70" s="3">
         <v>0</v>
@@ -8588,18 +8715,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:12">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>66</v>
       </c>
       <c r="B71" t="str">
-        <v>Noah Michael Alto</v>
+        <v>Sophia Joy Alto</v>
       </c>
       <c r="C71">
         <v>0</v>
       </c>
       <c r="D71" t="str">
-        <v>male</v>
+        <v>female</v>
       </c>
       <c r="E71" s="3">
         <v>0</v>
@@ -8608,10 +8735,10 @@
         <v>0</v>
       </c>
       <c r="G71">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H71">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I71" t="str">
         <v/>
@@ -8627,18 +8754,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:12">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>67</v>
       </c>
       <c r="B72" t="str">
-        <v>Marina Alto</v>
+        <v>Noah Michael Alto</v>
       </c>
       <c r="C72">
         <v>0</v>
       </c>
       <c r="D72" t="str">
-        <v>female</v>
+        <v>male</v>
       </c>
       <c r="E72" s="3">
         <v>0</v>
@@ -8647,10 +8774,10 @@
         <v>0</v>
       </c>
       <c r="G72">
-        <v>35</v>
-      </c>
-      <c r="H72" t="str">
-        <v/>
+        <v>32</v>
+      </c>
+      <c r="H72">
+        <v>33</v>
       </c>
       <c r="I72" t="str">
         <v/>
@@ -8666,18 +8793,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:12">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>68</v>
       </c>
       <c r="B73" t="str">
-        <v>Alexander Adam Alto</v>
+        <v>Marina Alto</v>
       </c>
       <c r="C73">
         <v>0</v>
       </c>
       <c r="D73" t="str">
-        <v>male</v>
+        <v>female</v>
       </c>
       <c r="E73" s="3">
         <v>0</v>
@@ -8705,12 +8832,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:12">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>69</v>
       </c>
       <c r="B74" t="str">
-        <v>Jayson Jordan Alto</v>
+        <v>Alexander Adam Alto</v>
       </c>
       <c r="C74">
         <v>0</v>
@@ -8744,18 +8871,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:12">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>70</v>
       </c>
       <c r="B75" t="str">
-        <v>Dianne Joy Zano</v>
+        <v>Jayson Jordan Alto</v>
       </c>
       <c r="C75">
         <v>0</v>
       </c>
       <c r="D75" t="str">
-        <v>female</v>
+        <v>male</v>
       </c>
       <c r="E75" s="3">
         <v>0</v>
@@ -8764,10 +8891,10 @@
         <v>0</v>
       </c>
       <c r="G75">
-        <v>39</v>
-      </c>
-      <c r="H75">
-        <v>40</v>
+        <v>35</v>
+      </c>
+      <c r="H75" t="str">
+        <v/>
       </c>
       <c r="I75" t="str">
         <v/>
@@ -8783,12 +8910,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:12">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>71</v>
       </c>
       <c r="B76" t="str">
-        <v>Arlene Reese Alto</v>
+        <v>Dianne Joy Zano</v>
       </c>
       <c r="C76">
         <v>0</v>
@@ -8803,10 +8930,10 @@
         <v>0</v>
       </c>
       <c r="G76">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="H76">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="I76" t="str">
         <v/>
@@ -8822,18 +8949,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:12">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>72</v>
       </c>
       <c r="B77" t="str">
-        <v>Arden Rhyle</v>
+        <v>Arlene Reese Alto</v>
       </c>
       <c r="C77">
         <v>0</v>
       </c>
       <c r="D77" t="str">
-        <v>male</v>
+        <v>female</v>
       </c>
       <c r="E77" s="3">
         <v>0</v>
@@ -8861,18 +8988,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:12">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>73</v>
       </c>
       <c r="B78" t="str">
-        <v>Janiyah Obilex</v>
+        <v>Arden Rhyle</v>
       </c>
       <c r="C78">
         <v>0</v>
       </c>
       <c r="D78" t="str">
-        <v>female</v>
+        <v>male</v>
       </c>
       <c r="E78" s="3">
         <v>0</v>
@@ -8881,10 +9008,10 @@
         <v>0</v>
       </c>
       <c r="G78">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H78">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I78" t="str">
         <v/>
@@ -8900,18 +9027,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:12">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>74</v>
       </c>
       <c r="B79" t="str">
-        <v>Justin Lhance Alto</v>
+        <v>Janiyah Obilex</v>
       </c>
       <c r="C79">
         <v>0</v>
       </c>
       <c r="D79" t="str">
-        <v>male</v>
+        <v>female</v>
       </c>
       <c r="E79" s="3">
         <v>0</v>
@@ -8920,10 +9047,10 @@
         <v>0</v>
       </c>
       <c r="G79">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H79">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I79" t="str">
         <v/>
@@ -8939,12 +9066,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:12">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>75</v>
       </c>
       <c r="B80" t="str">
-        <v>Joshua Landice Alto</v>
+        <v>Justin Lhance Alto</v>
       </c>
       <c r="C80">
         <v>0</v>
@@ -8978,12 +9105,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:12">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>76</v>
       </c>
       <c r="B81" t="str">
-        <v>Jairo Leslie Alto</v>
+        <v>Joshua Landice Alto</v>
       </c>
       <c r="C81">
         <v>0</v>
@@ -9017,18 +9144,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:12">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>77</v>
       </c>
       <c r="B82" t="str">
-        <v>Lyza Joelie Alto</v>
+        <v>Jairo Leslie Alto</v>
       </c>
       <c r="C82">
         <v>0</v>
       </c>
       <c r="D82" t="str">
-        <v>female</v>
+        <v>male</v>
       </c>
       <c r="E82" s="3">
         <v>0</v>
@@ -9056,12 +9183,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:12">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>78</v>
       </c>
       <c r="B83" t="str">
-        <v>Ryder Garland</v>
+        <v>Lyza Joelie Alto</v>
       </c>
       <c r="C83">
         <v>0</v>
@@ -9075,11 +9202,11 @@
       <c r="F83" s="3">
         <v>0</v>
       </c>
-      <c r="G83" t="str">
-        <v/>
+      <c r="G83">
+        <v>49</v>
       </c>
       <c r="H83">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I83" t="str">
         <v/>
@@ -9095,12 +9222,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:12">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>79</v>
       </c>
       <c r="B84" t="str">
-        <v>Alexis Mai Lim</v>
+        <v>Ryder Garland</v>
       </c>
       <c r="C84">
         <v>0</v>
@@ -9114,11 +9241,11 @@
       <c r="F84" s="3">
         <v>0</v>
       </c>
-      <c r="G84">
-        <v>52</v>
+      <c r="G84" t="str">
+        <v/>
       </c>
       <c r="H84">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I84" t="str">
         <v/>
@@ -9131,13 +9258,130 @@
         <v/>
       </c>
       <c r="L84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>80</v>
+      </c>
+      <c r="B85" t="str">
+        <v>Alexis Mei Lim</v>
+      </c>
+      <c r="C85">
+        <v>0</v>
+      </c>
+      <c r="D85" t="str">
+        <v>female</v>
+      </c>
+      <c r="E85" s="3">
+        <v>41817</v>
+      </c>
+      <c r="F85" s="3">
+        <v>0</v>
+      </c>
+      <c r="G85">
+        <v>52</v>
+      </c>
+      <c r="H85">
+        <v>53</v>
+      </c>
+      <c r="I85" t="str">
+        <v/>
+      </c>
+      <c r="J85" t="str">
+        <v/>
+      </c>
+      <c r="K85" t="str">
+        <f ca="1"/>
+        <v>11 years, 7 months, 5 days</v>
+      </c>
+      <c r="L85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>81</v>
+      </c>
+      <c r="B86" t="str">
+        <v>Samara Jia Lim</v>
+      </c>
+      <c r="C86">
+        <v>0</v>
+      </c>
+      <c r="D86" t="str">
+        <v>female</v>
+      </c>
+      <c r="E86" s="3">
+        <v>44335</v>
+      </c>
+      <c r="F86" s="3">
+        <v>45164</v>
+      </c>
+      <c r="G86">
+        <v>52</v>
+      </c>
+      <c r="H86">
+        <v>53</v>
+      </c>
+      <c r="I86" t="str">
+        <v/>
+      </c>
+      <c r="J86" t="str">
+        <v>2 years, 3 months, 7 days</v>
+      </c>
+      <c r="K86" t="str">
+        <f ca="1"/>
+        <v/>
+      </c>
+      <c r="L86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>82</v>
+      </c>
+      <c r="B87" t="str">
+        <v>Tamsyn Jie Lim</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
+      </c>
+      <c r="D87" t="str">
+        <v>female</v>
+      </c>
+      <c r="E87" s="3">
+        <v>45188</v>
+      </c>
+      <c r="F87" s="3">
+        <v>0</v>
+      </c>
+      <c r="G87">
+        <v>52</v>
+      </c>
+      <c r="H87">
+        <v>53</v>
+      </c>
+      <c r="I87" t="str">
+        <v/>
+      </c>
+      <c r="J87" t="str">
+        <v/>
+      </c>
+      <c r="K87" t="str">
+        <f ca="1"/>
+        <v>2 years, 4 months, 13 days</v>
+      </c>
+      <c r="L87">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="z2qPucUrqzpAbNrSN+cTXqXL9VmvHlBebf7zJLZukSo935FG2MWtQHQaAHBYBjvhorIZyzPuXgxNE9xi36mPtA==" saltValue="RQEcPLaOesrjkBOnJxq8Pw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="A6:L10000">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>NOT(ISBLANK(A6))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9156,30 +9400,30 @@
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>22</v>
       </c>

</xml_diff>